<commit_message>
Data updated by GitHub Bot (2020-06-01 12) (#70)
Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/output/snapshot/9c24c2d6-bc87-568a-aff3-c42f38603962.xlsx
+++ b/output/snapshot/9c24c2d6-bc87-568a-aff3-c42f38603962.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\dfs-srv1.fohm.local\common\Data\covid-19\Do-filer och analys\filer till dashboard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Data\covid-19\Do-filer och analys\filer till dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6470"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12880" windowHeight="7030" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Antal per dag region" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Totalt antal per region" sheetId="4" r:id="rId4"/>
     <sheet name="Totalt antal per kön" sheetId="5" r:id="rId5"/>
     <sheet name="Totalt antal per åldersgrupp" sheetId="6" r:id="rId6"/>
-    <sheet name="FOHM 31 May 2020" sheetId="7" r:id="rId7"/>
+    <sheet name="FOHM  1 Jun 2020" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -505,9 +505,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W119"/>
+  <dimension ref="A1:W120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:N1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
@@ -8897,55 +8899,55 @@
         <v>43982</v>
       </c>
       <c r="B119" s="2">
-        <v>31</v>
+        <v>198</v>
       </c>
       <c r="C119" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D119" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E119" s="2">
         <v>0</v>
       </c>
       <c r="F119" s="2">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="G119" s="2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H119" s="2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I119" s="2">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="J119" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K119" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L119" s="2">
         <v>0</v>
       </c>
       <c r="M119" s="2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="N119" s="2">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="O119" s="2">
         <v>0</v>
       </c>
       <c r="P119" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q119" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R119" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S119" s="2">
         <v>0</v>
@@ -8954,12 +8956,83 @@
         <v>0</v>
       </c>
       <c r="U119" s="2">
-        <v>4</v>
+        <v>83</v>
       </c>
       <c r="V119" s="2">
         <v>0</v>
       </c>
       <c r="W119" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:23">
+      <c r="A120" s="1">
+        <v>43983</v>
+      </c>
+      <c r="B120" s="2">
+        <v>105</v>
+      </c>
+      <c r="C120" s="2">
+        <v>0</v>
+      </c>
+      <c r="D120" s="2">
+        <v>0</v>
+      </c>
+      <c r="E120" s="2">
+        <v>0</v>
+      </c>
+      <c r="F120" s="2">
+        <v>0</v>
+      </c>
+      <c r="G120" s="2">
+        <v>1</v>
+      </c>
+      <c r="H120" s="2">
+        <v>0</v>
+      </c>
+      <c r="I120" s="2">
+        <v>0</v>
+      </c>
+      <c r="J120" s="2">
+        <v>0</v>
+      </c>
+      <c r="K120" s="2">
+        <v>0</v>
+      </c>
+      <c r="L120" s="2">
+        <v>0</v>
+      </c>
+      <c r="M120" s="2">
+        <v>1</v>
+      </c>
+      <c r="N120" s="2">
+        <v>36</v>
+      </c>
+      <c r="O120" s="2">
+        <v>9</v>
+      </c>
+      <c r="P120" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q120" s="2">
+        <v>0</v>
+      </c>
+      <c r="R120" s="2">
+        <v>0</v>
+      </c>
+      <c r="S120" s="2">
+        <v>5</v>
+      </c>
+      <c r="T120" s="2">
+        <v>9</v>
+      </c>
+      <c r="U120" s="2">
+        <v>44</v>
+      </c>
+      <c r="V120" s="2">
+        <v>0</v>
+      </c>
+      <c r="W120" s="2">
         <v>0</v>
       </c>
     </row>
@@ -8970,10 +9043,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B82"/>
+  <dimension ref="A1:B85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F68" sqref="F68"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="A73" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -9626,14 +9699,38 @@
         <v>43980</v>
       </c>
       <c r="B81" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="82" spans="1:2">
-      <c r="A82" s="1" t="s">
+      <c r="A82" s="1">
+        <v>43981</v>
+      </c>
+      <c r="B82" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="1">
+        <v>43982</v>
+      </c>
+      <c r="B83" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="1">
+        <v>43983</v>
+      </c>
+      <c r="B84" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B82" s="2">
+      <c r="B85" s="2">
         <v>11</v>
       </c>
     </row>
@@ -9644,9 +9741,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B88"/>
+  <dimension ref="A1:B89"/>
   <sheetViews>
-    <sheetView topLeftCell="A69" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
@@ -10242,7 +10341,7 @@
         <v>43968</v>
       </c>
       <c r="B74" s="2">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -10330,7 +10429,7 @@
         <v>43979</v>
       </c>
       <c r="B85" s="2">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -10338,7 +10437,7 @@
         <v>43980</v>
       </c>
       <c r="B86" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -10346,7 +10445,7 @@
         <v>43981</v>
       </c>
       <c r="B87" s="2">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -10354,7 +10453,15 @@
         <v>43982</v>
       </c>
       <c r="B88" s="2">
-        <v>3</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" s="1">
+        <v>43983</v>
+      </c>
+      <c r="B89" s="2">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -10366,11 +10473,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -10394,10 +10506,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="2">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="C2" s="2">
-        <v>130.3209228515625</v>
+        <v>132.20054626464844</v>
       </c>
       <c r="D2" s="2">
         <v>3</v>
@@ -10411,10 +10523,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>1215</v>
+        <v>1217</v>
       </c>
       <c r="C3" s="2">
-        <v>421.9248046875</v>
+        <v>422.61932373046875</v>
       </c>
       <c r="D3" s="2">
         <v>58</v>
@@ -10445,13 +10557,13 @@
         <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>1285</v>
+        <v>1293</v>
       </c>
       <c r="C5" s="2">
-        <v>447.14004516601563</v>
+        <v>449.92379760742188</v>
       </c>
       <c r="D5" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E5" s="2">
         <v>103</v>
@@ -10462,10 +10574,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="2">
-        <v>773</v>
+        <v>781</v>
       </c>
       <c r="C6" s="2">
-        <v>231.54249572753906</v>
+        <v>233.93879699707031</v>
       </c>
       <c r="D6" s="2">
         <v>30</v>
@@ -10479,10 +10591,10 @@
         <v>28</v>
       </c>
       <c r="B7" s="2">
-        <v>722</v>
+        <v>729</v>
       </c>
       <c r="C7" s="2">
-        <v>551.945556640625</v>
+        <v>557.29681396484375</v>
       </c>
       <c r="D7" s="2">
         <v>15</v>
@@ -10496,16 +10608,16 @@
         <v>8</v>
       </c>
       <c r="B8" s="2">
-        <v>1538</v>
+        <v>1554</v>
       </c>
       <c r="C8" s="2">
-        <v>422.99346923828125</v>
+        <v>427.3939208984375</v>
       </c>
       <c r="D8" s="2">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E8" s="2">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -10513,10 +10625,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="2">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="C9" s="2">
-        <v>142.19013977050781</v>
+        <v>143.41239929199219</v>
       </c>
       <c r="D9" s="2">
         <v>23</v>
@@ -10530,10 +10642,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="2">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="C10" s="2">
-        <v>416.44125366210938</v>
+        <v>416.93759155273438</v>
       </c>
       <c r="D10" s="2">
         <v>17</v>
@@ -10564,13 +10676,13 @@
         <v>12</v>
       </c>
       <c r="B12" s="2">
-        <v>1739</v>
+        <v>1747</v>
       </c>
       <c r="C12" s="2">
-        <v>126.21323394775391</v>
+        <v>126.79385375976563</v>
       </c>
       <c r="D12" s="2">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E12" s="2">
         <v>178</v>
@@ -10581,16 +10693,16 @@
         <v>13</v>
       </c>
       <c r="B13" s="2">
-        <v>12149</v>
+        <v>12208</v>
       </c>
       <c r="C13" s="2">
-        <v>511.08901977539063</v>
+        <v>513.571044921875</v>
       </c>
       <c r="D13" s="2">
-        <v>790</v>
+        <v>797</v>
       </c>
       <c r="E13" s="2">
-        <v>2055</v>
+        <v>2058</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -10598,13 +10710,13 @@
         <v>14</v>
       </c>
       <c r="B14" s="2">
-        <v>1625</v>
+        <v>1634</v>
       </c>
       <c r="C14" s="2">
-        <v>546.14508056640625</v>
+        <v>549.16986083984375</v>
       </c>
       <c r="D14" s="2">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E14" s="2">
         <v>224</v>
@@ -10615,13 +10727,13 @@
         <v>15</v>
       </c>
       <c r="B15" s="2">
-        <v>1921</v>
+        <v>1929</v>
       </c>
       <c r="C15" s="2">
-        <v>500.63458251953125</v>
+        <v>502.719482421875</v>
       </c>
       <c r="D15" s="2">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="E15" s="2">
         <v>169</v>
@@ -10632,16 +10744,16 @@
         <v>16</v>
       </c>
       <c r="B16" s="2">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="C16" s="2">
-        <v>188.02183532714844</v>
+        <v>188.37593078613281</v>
       </c>
       <c r="D16" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E16" s="2">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -10649,10 +10761,10 @@
         <v>17</v>
       </c>
       <c r="B17" s="2">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="C17" s="2">
-        <v>183.26611328125</v>
+        <v>184.00212097167969</v>
       </c>
       <c r="D17" s="2">
         <v>28</v>
@@ -10666,10 +10778,10 @@
         <v>18</v>
       </c>
       <c r="B18" s="2">
-        <v>723</v>
+        <v>728</v>
       </c>
       <c r="C18" s="2">
-        <v>294.68466186523438</v>
+        <v>296.72259521484375</v>
       </c>
       <c r="D18" s="2">
         <v>39</v>
@@ -10683,10 +10795,10 @@
         <v>19</v>
       </c>
       <c r="B19" s="2">
-        <v>1264</v>
+        <v>1273</v>
       </c>
       <c r="C19" s="2">
-        <v>458.22836303710938</v>
+        <v>461.49105834960938</v>
       </c>
       <c r="D19" s="2">
         <v>44</v>
@@ -10700,16 +10812,16 @@
         <v>29</v>
       </c>
       <c r="B20" s="2">
-        <v>5898</v>
+        <v>6021</v>
       </c>
       <c r="C20" s="2">
-        <v>341.73849487304688</v>
+        <v>348.86529541015625</v>
       </c>
       <c r="D20" s="2">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="E20" s="2">
-        <v>550</v>
+        <v>551</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -10726,7 +10838,7 @@
         <v>71</v>
       </c>
       <c r="E21" s="2">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -10740,7 +10852,7 @@
         <v>424.279541015625</v>
       </c>
       <c r="D22" s="2">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E22" s="2">
         <v>190</v>
@@ -10778,13 +10890,13 @@
         <v>34</v>
       </c>
       <c r="B2" s="2">
-        <v>15295</v>
+        <v>15395</v>
       </c>
       <c r="C2" s="2">
-        <v>1526</v>
+        <v>1539</v>
       </c>
       <c r="D2" s="2">
-        <v>2418</v>
+        <v>2421</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -10792,13 +10904,13 @@
         <v>35</v>
       </c>
       <c r="B3" s="2">
-        <v>22247</v>
+        <v>22419</v>
       </c>
       <c r="C3" s="2">
-        <v>538</v>
+        <v>544</v>
       </c>
       <c r="D3" s="2">
-        <v>1977</v>
+        <v>1982</v>
       </c>
     </row>
   </sheetData>
@@ -10810,11 +10922,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="13.08984375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -10835,7 +10948,7 @@
         <v>37</v>
       </c>
       <c r="B2" s="2">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C2" s="2">
         <v>4</v>
@@ -10849,7 +10962,7 @@
         <v>38</v>
       </c>
       <c r="B3" s="2">
-        <v>454</v>
+        <v>457</v>
       </c>
       <c r="C3" s="2">
         <v>7</v>
@@ -10863,10 +10976,10 @@
         <v>39</v>
       </c>
       <c r="B4" s="2">
-        <v>3492</v>
+        <v>3527</v>
       </c>
       <c r="C4" s="2">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D4" s="2">
         <v>8</v>
@@ -10877,10 +10990,10 @@
         <v>40</v>
       </c>
       <c r="B5" s="2">
-        <v>4544</v>
+        <v>4585</v>
       </c>
       <c r="C5" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D5" s="2">
         <v>12</v>
@@ -10891,10 +11004,10 @@
         <v>41</v>
       </c>
       <c r="B6" s="2">
-        <v>5508</v>
+        <v>5566</v>
       </c>
       <c r="C6" s="2">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="D6" s="2">
         <v>42</v>
@@ -10905,10 +11018,10 @@
         <v>42</v>
       </c>
       <c r="B7" s="2">
-        <v>6810</v>
+        <v>6869</v>
       </c>
       <c r="C7" s="2">
-        <v>544</v>
+        <v>551</v>
       </c>
       <c r="D7" s="2">
         <v>132</v>
@@ -10919,10 +11032,10 @@
         <v>43</v>
       </c>
       <c r="B8" s="2">
-        <v>4552</v>
+        <v>4592</v>
       </c>
       <c r="C8" s="2">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D8" s="2">
         <v>311</v>
@@ -10933,13 +11046,13 @@
         <v>44</v>
       </c>
       <c r="B9" s="2">
-        <v>4104</v>
+        <v>4112</v>
       </c>
       <c r="C9" s="2">
-        <v>401</v>
+        <v>407</v>
       </c>
       <c r="D9" s="2">
-        <v>963</v>
+        <v>967</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -10947,13 +11060,13 @@
         <v>45</v>
       </c>
       <c r="B10" s="2">
-        <v>5087</v>
+        <v>5102</v>
       </c>
       <c r="C10" s="2">
         <v>80</v>
       </c>
       <c r="D10" s="2">
-        <v>1813</v>
+        <v>1815</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -10961,13 +11074,13 @@
         <v>46</v>
       </c>
       <c r="B11" s="2">
-        <v>2802</v>
+        <v>2810</v>
       </c>
       <c r="C11" s="2">
         <v>1</v>
       </c>
       <c r="D11" s="2">
-        <v>1113</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -10975,7 +11088,7 @@
         <v>47</v>
       </c>
       <c r="B12" s="2">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C12" s="2">
         <v>0</v>
@@ -10993,7 +11106,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-04 12) (#79)
Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/output/snapshot/9c24c2d6-bc87-568a-aff3-c42f38603962.xlsx
+++ b/output/snapshot/9c24c2d6-bc87-568a-aff3-c42f38603962.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14316" windowHeight="6912" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Antal per dag region" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Totalt antal per region" sheetId="4" r:id="rId4"/>
     <sheet name="Totalt antal per kön" sheetId="5" r:id="rId5"/>
     <sheet name="Totalt antal per åldersgrupp" sheetId="6" r:id="rId6"/>
-    <sheet name="FOHM  3 Jun 2020" sheetId="7" r:id="rId7"/>
+    <sheet name="FOHM  4 Jun 2020" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -505,13 +505,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W122"/>
+  <dimension ref="A1:W123"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B24" sqref="B1:B1048576"/>
+    <sheetView topLeftCell="A102" workbookViewId="0">
+      <selection activeCell="B102" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="13.54296875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:23">
       <c r="A1" t="s">
@@ -5914,7 +5917,7 @@
         <v>43940</v>
       </c>
       <c r="B77" s="2">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C77" s="2">
         <v>0</v>
@@ -5956,7 +5959,7 @@
         <v>13</v>
       </c>
       <c r="P77" s="2">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q77" s="2">
         <v>4</v>
@@ -9109,70 +9112,141 @@
         <v>43985</v>
       </c>
       <c r="B122" s="2">
-        <v>157</v>
+        <v>1044</v>
       </c>
       <c r="C122" s="2">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="D122" s="2">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="E122" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F122" s="2">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="G122" s="2">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H122" s="2">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="I122" s="2">
+        <v>41</v>
+      </c>
+      <c r="J122" s="2">
+        <v>9</v>
+      </c>
+      <c r="K122" s="2">
+        <v>12</v>
+      </c>
+      <c r="L122" s="2">
+        <v>15</v>
+      </c>
+      <c r="M122" s="2">
+        <v>38</v>
+      </c>
+      <c r="N122" s="2">
+        <v>234</v>
+      </c>
+      <c r="O122" s="2">
+        <v>2</v>
+      </c>
+      <c r="P122" s="2">
+        <v>50</v>
+      </c>
+      <c r="Q122" s="2">
+        <v>14</v>
+      </c>
+      <c r="R122" s="2">
+        <v>5</v>
+      </c>
+      <c r="S122" s="2">
+        <v>28</v>
+      </c>
+      <c r="T122" s="2">
+        <v>33</v>
+      </c>
+      <c r="U122" s="2">
+        <v>421</v>
+      </c>
+      <c r="V122" s="2">
+        <v>24</v>
+      </c>
+      <c r="W122" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="123" spans="1:23">
+      <c r="A123" s="1">
+        <v>43986</v>
+      </c>
+      <c r="B123" s="2">
+        <v>194</v>
+      </c>
+      <c r="C123" s="2">
+        <v>0</v>
+      </c>
+      <c r="D123" s="2">
+        <v>0</v>
+      </c>
+      <c r="E123" s="2">
+        <v>0</v>
+      </c>
+      <c r="F123" s="2">
+        <v>17</v>
+      </c>
+      <c r="G123" s="2">
+        <v>0</v>
+      </c>
+      <c r="H123" s="2">
+        <v>4</v>
+      </c>
+      <c r="I123" s="2">
+        <v>4</v>
+      </c>
+      <c r="J123" s="2">
+        <v>0</v>
+      </c>
+      <c r="K123" s="2">
+        <v>1</v>
+      </c>
+      <c r="L123" s="2">
+        <v>1</v>
+      </c>
+      <c r="M123" s="2">
         <v>11</v>
       </c>
-      <c r="J122" s="2">
-        <v>0</v>
-      </c>
-      <c r="K122" s="2">
-        <v>0</v>
-      </c>
-      <c r="L122" s="2">
-        <v>3</v>
-      </c>
-      <c r="M122" s="2">
-        <v>5</v>
-      </c>
-      <c r="N122" s="2">
-        <v>36</v>
-      </c>
-      <c r="O122" s="2">
-        <v>2</v>
-      </c>
-      <c r="P122" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q122" s="2">
+      <c r="N123" s="2">
+        <v>33</v>
+      </c>
+      <c r="O123" s="2">
+        <v>2</v>
+      </c>
+      <c r="P123" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q123" s="2">
+        <v>8</v>
+      </c>
+      <c r="R123" s="2">
+        <v>0</v>
+      </c>
+      <c r="S123" s="2">
         <v>4</v>
       </c>
-      <c r="R122" s="2">
-        <v>0</v>
-      </c>
-      <c r="S122" s="2">
-        <v>11</v>
-      </c>
-      <c r="T122" s="2">
-        <v>15</v>
-      </c>
-      <c r="U122" s="2">
-        <v>60</v>
-      </c>
-      <c r="V122" s="2">
+      <c r="T123" s="2">
+        <v>16</v>
+      </c>
+      <c r="U123" s="2">
+        <v>58</v>
+      </c>
+      <c r="V123" s="2">
         <v>6</v>
       </c>
-      <c r="W122" s="2">
-        <v>0</v>
+      <c r="W123" s="2">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -9182,13 +9256,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B87"/>
+  <dimension ref="A1:B88"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="B82" sqref="B1:B1048576"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A88" sqref="A88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="12.26953125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -9779,7 +9856,7 @@
         <v>43973</v>
       </c>
       <c r="B74" s="2">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -9787,7 +9864,7 @@
         <v>43974</v>
       </c>
       <c r="B75" s="2">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -9803,7 +9880,7 @@
         <v>43976</v>
       </c>
       <c r="B77" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -9819,7 +9896,7 @@
         <v>43978</v>
       </c>
       <c r="B79" s="2">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -9827,7 +9904,7 @@
         <v>43979</v>
       </c>
       <c r="B80" s="2">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -9843,7 +9920,7 @@
         <v>43981</v>
       </c>
       <c r="B82" s="2">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -9851,7 +9928,7 @@
         <v>43982</v>
       </c>
       <c r="B83" s="2">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -9859,7 +9936,7 @@
         <v>43983</v>
       </c>
       <c r="B84" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -9867,7 +9944,7 @@
         <v>43984</v>
       </c>
       <c r="B85" s="2">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -9875,14 +9952,22 @@
         <v>43985</v>
       </c>
       <c r="B86" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="87" spans="1:2">
-      <c r="A87" s="1" t="s">
+      <c r="A87" s="1">
+        <v>43986</v>
+      </c>
+      <c r="B87" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B87" s="2">
+      <c r="B88" s="2">
         <v>11</v>
       </c>
     </row>
@@ -9893,13 +9978,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B91"/>
+  <dimension ref="A1:B92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -10218,7 +10303,7 @@
         <v>43934</v>
       </c>
       <c r="B40" s="2">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -10226,7 +10311,7 @@
         <v>43935</v>
       </c>
       <c r="B41" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -10242,7 +10327,7 @@
         <v>43937</v>
       </c>
       <c r="B43" s="2">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -10586,7 +10671,7 @@
         <v>43980</v>
       </c>
       <c r="B86" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -10594,7 +10679,7 @@
         <v>43981</v>
       </c>
       <c r="B87" s="2">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -10610,7 +10695,7 @@
         <v>43983</v>
       </c>
       <c r="B89" s="2">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -10618,7 +10703,7 @@
         <v>43984</v>
       </c>
       <c r="B90" s="2">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -10626,7 +10711,15 @@
         <v>43985</v>
       </c>
       <c r="B91" s="2">
-        <v>3</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" s="1">
+        <v>43986</v>
+      </c>
+      <c r="B92" s="2">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -10642,7 +10735,7 @@
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -10666,13 +10759,13 @@
         <v>2</v>
       </c>
       <c r="B2" s="2">
-        <v>236</v>
+        <v>254</v>
       </c>
       <c r="C2" s="2">
-        <v>147.86412048339844</v>
+        <v>159.14189147949219</v>
       </c>
       <c r="D2" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E2" s="2">
         <v>5</v>
@@ -10683,10 +10776,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>1250</v>
+        <v>1264</v>
       </c>
       <c r="C3" s="2">
-        <v>434.07901000976563</v>
+        <v>438.94070434570313</v>
       </c>
       <c r="D3" s="2">
         <v>60</v>
@@ -10700,10 +10793,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C4" s="2">
-        <v>144.08738708496094</v>
+        <v>145.76283264160156</v>
       </c>
       <c r="D4" s="2">
         <v>5</v>
@@ -10717,13 +10810,13 @@
         <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>1351</v>
+        <v>1400</v>
       </c>
       <c r="C5" s="2">
-        <v>470.10598754882813</v>
+        <v>487.15646362304688</v>
       </c>
       <c r="D5" s="2">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E5" s="2">
         <v>109</v>
@@ -10734,10 +10827,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="2">
-        <v>833</v>
+        <v>843</v>
       </c>
       <c r="C6" s="2">
-        <v>249.51475524902344</v>
+        <v>252.5101318359375</v>
       </c>
       <c r="D6" s="2">
         <v>30</v>
@@ -10751,10 +10844,10 @@
         <v>28</v>
       </c>
       <c r="B7" s="2">
-        <v>744</v>
+        <v>757</v>
       </c>
       <c r="C7" s="2">
-        <v>568.76385498046875</v>
+        <v>578.701904296875</v>
       </c>
       <c r="D7" s="2">
         <v>15</v>
@@ -10768,16 +10861,16 @@
         <v>8</v>
       </c>
       <c r="B8" s="2">
-        <v>1613</v>
+        <v>1647</v>
       </c>
       <c r="C8" s="2">
-        <v>443.62057495117188</v>
+        <v>452.9715576171875</v>
       </c>
       <c r="D8" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E8" s="2">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -10785,13 +10878,13 @@
         <v>9</v>
       </c>
       <c r="B9" s="2">
-        <v>367</v>
+        <v>376</v>
       </c>
       <c r="C9" s="2">
-        <v>149.52372741699219</v>
+        <v>153.19052124023438</v>
       </c>
       <c r="D9" s="2">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E9" s="2">
         <v>36</v>
@@ -10802,16 +10895,16 @@
         <v>10</v>
       </c>
       <c r="B10" s="2">
-        <v>873</v>
+        <v>886</v>
       </c>
       <c r="C10" s="2">
-        <v>433.31729125976563</v>
+        <v>439.7698974609375</v>
       </c>
       <c r="D10" s="2">
         <v>17</v>
       </c>
       <c r="E10" s="2">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -10819,16 +10912,16 @@
         <v>11</v>
       </c>
       <c r="B11" s="2">
-        <v>448</v>
+        <v>461</v>
       </c>
       <c r="C11" s="2">
-        <v>179.13336181640625</v>
+        <v>184.33143615722656</v>
       </c>
       <c r="D11" s="2">
         <v>37</v>
       </c>
       <c r="E11" s="2">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -10836,16 +10929,16 @@
         <v>12</v>
       </c>
       <c r="B12" s="2">
-        <v>1848</v>
+        <v>1892</v>
       </c>
       <c r="C12" s="2">
-        <v>134.12423706054688</v>
+        <v>137.31767272949219</v>
       </c>
       <c r="D12" s="2">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E12" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -10853,16 +10946,16 @@
         <v>13</v>
       </c>
       <c r="B13" s="2">
-        <v>13877</v>
+        <v>14108</v>
       </c>
       <c r="C13" s="2">
-        <v>583.783203125</v>
+        <v>593.50103759765625</v>
       </c>
       <c r="D13" s="2">
-        <v>811</v>
+        <v>815</v>
       </c>
       <c r="E13" s="2">
-        <v>2099</v>
+        <v>2103</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -10870,10 +10963,10 @@
         <v>14</v>
       </c>
       <c r="B14" s="2">
-        <v>1641</v>
+        <v>1643</v>
       </c>
       <c r="C14" s="2">
-        <v>551.5224609375</v>
+        <v>552.19464111328125</v>
       </c>
       <c r="D14" s="2">
         <v>125</v>
@@ -10887,13 +10980,13 @@
         <v>15</v>
       </c>
       <c r="B15" s="2">
-        <v>2029</v>
+        <v>2077</v>
       </c>
       <c r="C15" s="2">
-        <v>528.7806396484375</v>
+        <v>541.28997802734375</v>
       </c>
       <c r="D15" s="2">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E15" s="2">
         <v>182</v>
@@ -10904,16 +10997,16 @@
         <v>16</v>
       </c>
       <c r="B16" s="2">
-        <v>564</v>
+        <v>582</v>
       </c>
       <c r="C16" s="2">
-        <v>199.70681762695313</v>
+        <v>206.08042907714844</v>
       </c>
       <c r="D16" s="2">
         <v>23</v>
       </c>
       <c r="E16" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -10921,10 +11014,10 @@
         <v>17</v>
       </c>
       <c r="B17" s="2">
-        <v>508</v>
+        <v>513</v>
       </c>
       <c r="C17" s="2">
-        <v>186.94615173339844</v>
+        <v>188.78617858886719</v>
       </c>
       <c r="D17" s="2">
         <v>28</v>
@@ -10938,10 +11031,10 @@
         <v>18</v>
       </c>
       <c r="B18" s="2">
-        <v>785</v>
+        <v>806</v>
       </c>
       <c r="C18" s="2">
-        <v>319.95501708984375</v>
+        <v>328.51431274414063</v>
       </c>
       <c r="D18" s="2">
         <v>40</v>
@@ -10955,10 +11048,10 @@
         <v>19</v>
       </c>
       <c r="B19" s="2">
-        <v>1367</v>
+        <v>1401</v>
       </c>
       <c r="C19" s="2">
-        <v>495.56817626953125</v>
+        <v>507.8939208984375</v>
       </c>
       <c r="D19" s="2">
         <v>44</v>
@@ -10972,16 +11065,16 @@
         <v>29</v>
       </c>
       <c r="B20" s="2">
-        <v>6414</v>
+        <v>6833</v>
       </c>
       <c r="C20" s="2">
-        <v>371.63629150390625</v>
+        <v>395.91372680664063</v>
       </c>
       <c r="D20" s="2">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="E20" s="2">
-        <v>579</v>
+        <v>582</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -10989,16 +11082,16 @@
         <v>21</v>
       </c>
       <c r="B21" s="2">
-        <v>1870</v>
+        <v>1894</v>
       </c>
       <c r="C21" s="2">
-        <v>613.50701904296875</v>
+        <v>621.380859375</v>
       </c>
       <c r="D21" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E21" s="2">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -11006,16 +11099,16 @@
         <v>22</v>
       </c>
       <c r="B22" s="2">
-        <v>2099</v>
+        <v>2159</v>
       </c>
       <c r="C22" s="2">
-        <v>450.9178466796875</v>
+        <v>463.80734252929688</v>
       </c>
       <c r="D22" s="2">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E22" s="2">
-        <v>190</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -11031,7 +11124,7 @@
       <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -11052,13 +11145,13 @@
         <v>34</v>
       </c>
       <c r="B2" s="2">
-        <v>16259</v>
+        <v>16631</v>
       </c>
       <c r="C2" s="2">
-        <v>1565</v>
+        <v>1579</v>
       </c>
       <c r="D2" s="2">
-        <v>2489</v>
+        <v>2503</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -11066,13 +11159,13 @@
         <v>35</v>
       </c>
       <c r="B3" s="2">
-        <v>24543</v>
+        <v>25251</v>
       </c>
       <c r="C3" s="2">
-        <v>556</v>
+        <v>564</v>
       </c>
       <c r="D3" s="2">
-        <v>2053</v>
+        <v>2059</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -11098,11 +11191,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -11123,7 +11216,7 @@
         <v>38</v>
       </c>
       <c r="B2" s="2">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="C2" s="2">
         <v>5</v>
@@ -11137,7 +11230,7 @@
         <v>39</v>
       </c>
       <c r="B3" s="2">
-        <v>497</v>
+        <v>518</v>
       </c>
       <c r="C3" s="2">
         <v>9</v>
@@ -11151,7 +11244,7 @@
         <v>40</v>
       </c>
       <c r="B4" s="2">
-        <v>3909</v>
+        <v>4058</v>
       </c>
       <c r="C4" s="2">
         <v>79</v>
@@ -11165,13 +11258,13 @@
         <v>41</v>
       </c>
       <c r="B5" s="2">
-        <v>5239</v>
+        <v>5433</v>
       </c>
       <c r="C5" s="2">
         <v>95</v>
       </c>
       <c r="D5" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -11179,10 +11272,10 @@
         <v>42</v>
       </c>
       <c r="B6" s="2">
-        <v>6240</v>
+        <v>6463</v>
       </c>
       <c r="C6" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D6" s="2">
         <v>42</v>
@@ -11193,10 +11286,10 @@
         <v>43</v>
       </c>
       <c r="B7" s="2">
-        <v>7489</v>
+        <v>7705</v>
       </c>
       <c r="C7" s="2">
-        <v>562</v>
+        <v>565</v>
       </c>
       <c r="D7" s="2">
         <v>134</v>
@@ -11207,13 +11300,13 @@
         <v>44</v>
       </c>
       <c r="B8" s="2">
-        <v>4903</v>
+        <v>5020</v>
       </c>
       <c r="C8" s="2">
-        <v>631</v>
+        <v>643</v>
       </c>
       <c r="D8" s="2">
-        <v>321</v>
+        <v>324</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -11221,13 +11314,13 @@
         <v>45</v>
       </c>
       <c r="B9" s="2">
-        <v>4223</v>
+        <v>4288</v>
       </c>
       <c r="C9" s="2">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="D9" s="2">
-        <v>998</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -11235,13 +11328,13 @@
         <v>46</v>
       </c>
       <c r="B10" s="2">
-        <v>5227</v>
+        <v>5284</v>
       </c>
       <c r="C10" s="2">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D10" s="2">
-        <v>1867</v>
+        <v>1874</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -11249,13 +11342,13 @@
         <v>47</v>
       </c>
       <c r="B11" s="2">
-        <v>2871</v>
+        <v>2903</v>
       </c>
       <c r="C11" s="2">
         <v>1</v>
       </c>
       <c r="D11" s="2">
-        <v>1158</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -11263,7 +11356,7 @@
         <v>36</v>
       </c>
       <c r="B12" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C12" s="2">
         <v>0</v>
@@ -11281,11 +11374,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-05 12:09)
</commit_message>
<xml_diff>
--- a/output/snapshot/9c24c2d6-bc87-568a-aff3-c42f38603962.xlsx
+++ b/output/snapshot/9c24c2d6-bc87-568a-aff3-c42f38603962.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Antal per dag region" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Totalt antal per region" sheetId="4" r:id="rId4"/>
     <sheet name="Totalt antal per kön" sheetId="5" r:id="rId5"/>
     <sheet name="Totalt antal per åldersgrupp" sheetId="6" r:id="rId6"/>
-    <sheet name="FOHM  4 Jun 2020" sheetId="7" r:id="rId7"/>
+    <sheet name="FOHM  5 Jun 2020" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -505,15 +505,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W123"/>
+  <dimension ref="A1:W124"/>
   <sheetViews>
-    <sheetView topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="B102" sqref="B1:B1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.54296875" customWidth="1"/>
+    <col min="1" max="1" width="12.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
@@ -3929,7 +3929,7 @@
         <v>43912</v>
       </c>
       <c r="B49" s="2">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C49" s="2">
         <v>0</v>
@@ -3959,7 +3959,7 @@
         <v>0</v>
       </c>
       <c r="L49" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M49" s="2">
         <v>3</v>
@@ -5562,7 +5562,7 @@
         <v>43935</v>
       </c>
       <c r="B72" s="2">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C72" s="2">
         <v>1</v>
@@ -5583,7 +5583,7 @@
         <v>14</v>
       </c>
       <c r="I72" s="2">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J72" s="2">
         <v>5</v>
@@ -8598,10 +8598,10 @@
         <v>41</v>
       </c>
       <c r="T114" s="2">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="U114" s="2">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="V114" s="2">
         <v>28</v>
@@ -8713,13 +8713,13 @@
         <v>18</v>
       </c>
       <c r="K116" s="2">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L116" s="2">
         <v>6</v>
       </c>
       <c r="M116" s="2">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N116" s="2">
         <v>282</v>
@@ -9112,7 +9112,7 @@
         <v>43985</v>
       </c>
       <c r="B122" s="2">
-        <v>1044</v>
+        <v>1070</v>
       </c>
       <c r="C122" s="2">
         <v>18</v>
@@ -9124,7 +9124,7 @@
         <v>1</v>
       </c>
       <c r="F122" s="2">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G122" s="2">
         <v>11</v>
@@ -9148,10 +9148,10 @@
         <v>38</v>
       </c>
       <c r="N122" s="2">
-        <v>234</v>
+        <v>250</v>
       </c>
       <c r="O122" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P122" s="2">
         <v>50</v>
@@ -9163,13 +9163,13 @@
         <v>5</v>
       </c>
       <c r="S122" s="2">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="T122" s="2">
         <v>33</v>
       </c>
       <c r="U122" s="2">
-        <v>421</v>
+        <v>429</v>
       </c>
       <c r="V122" s="2">
         <v>24</v>
@@ -9183,70 +9183,141 @@
         <v>43986</v>
       </c>
       <c r="B123" s="2">
-        <v>194</v>
+        <v>997</v>
       </c>
       <c r="C123" s="2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D123" s="2">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E123" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F123" s="2">
+        <v>44</v>
+      </c>
+      <c r="G123" s="2">
+        <v>22</v>
+      </c>
+      <c r="H123" s="2">
+        <v>15</v>
+      </c>
+      <c r="I123" s="2">
+        <v>26</v>
+      </c>
+      <c r="J123" s="2">
+        <v>14</v>
+      </c>
+      <c r="K123" s="2">
+        <v>11</v>
+      </c>
+      <c r="L123" s="2">
+        <v>19</v>
+      </c>
+      <c r="M123" s="2">
+        <v>42</v>
+      </c>
+      <c r="N123" s="2">
+        <v>219</v>
+      </c>
+      <c r="O123" s="2">
+        <v>12</v>
+      </c>
+      <c r="P123" s="2">
+        <v>57</v>
+      </c>
+      <c r="Q123" s="2">
+        <v>21</v>
+      </c>
+      <c r="R123" s="2">
+        <v>5</v>
+      </c>
+      <c r="S123" s="2">
+        <v>25</v>
+      </c>
+      <c r="T123" s="2">
+        <v>33</v>
+      </c>
+      <c r="U123" s="2">
+        <v>363</v>
+      </c>
+      <c r="V123" s="2">
+        <v>8</v>
+      </c>
+      <c r="W123" s="2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="124" spans="1:23">
+      <c r="A124" s="1">
+        <v>43987</v>
+      </c>
+      <c r="B124" s="2">
+        <v>227</v>
+      </c>
+      <c r="C124" s="2">
+        <v>0</v>
+      </c>
+      <c r="D124" s="2">
+        <v>0</v>
+      </c>
+      <c r="E124" s="2">
+        <v>0</v>
+      </c>
+      <c r="F124" s="2">
+        <v>9</v>
+      </c>
+      <c r="G124" s="2">
+        <v>5</v>
+      </c>
+      <c r="H124" s="2">
+        <v>6</v>
+      </c>
+      <c r="I124" s="2">
+        <v>13</v>
+      </c>
+      <c r="J124" s="2">
+        <v>0</v>
+      </c>
+      <c r="K124" s="2">
+        <v>0</v>
+      </c>
+      <c r="L124" s="2">
+        <v>1</v>
+      </c>
+      <c r="M124" s="2">
+        <v>6</v>
+      </c>
+      <c r="N124" s="2">
+        <v>56</v>
+      </c>
+      <c r="O124" s="2">
+        <v>1</v>
+      </c>
+      <c r="P124" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q124" s="2">
+        <v>4</v>
+      </c>
+      <c r="R124" s="2">
+        <v>0</v>
+      </c>
+      <c r="S124" s="2">
+        <v>6</v>
+      </c>
+      <c r="T124" s="2">
         <v>17</v>
       </c>
-      <c r="G123" s="2">
-        <v>0</v>
-      </c>
-      <c r="H123" s="2">
-        <v>4</v>
-      </c>
-      <c r="I123" s="2">
-        <v>4</v>
-      </c>
-      <c r="J123" s="2">
-        <v>0</v>
-      </c>
-      <c r="K123" s="2">
-        <v>1</v>
-      </c>
-      <c r="L123" s="2">
-        <v>1</v>
-      </c>
-      <c r="M123" s="2">
-        <v>11</v>
-      </c>
-      <c r="N123" s="2">
-        <v>33</v>
-      </c>
-      <c r="O123" s="2">
-        <v>2</v>
-      </c>
-      <c r="P123" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q123" s="2">
-        <v>8</v>
-      </c>
-      <c r="R123" s="2">
-        <v>0</v>
-      </c>
-      <c r="S123" s="2">
-        <v>4</v>
-      </c>
-      <c r="T123" s="2">
-        <v>16</v>
-      </c>
-      <c r="U123" s="2">
-        <v>58</v>
-      </c>
-      <c r="V123" s="2">
-        <v>6</v>
-      </c>
-      <c r="W123" s="2">
-        <v>29</v>
+      <c r="U124" s="2">
+        <v>71</v>
+      </c>
+      <c r="V124" s="2">
+        <v>0</v>
+      </c>
+      <c r="W124" s="2">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -9258,13 +9329,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B88"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="A88" sqref="A88"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="B85" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="12.26953125" customWidth="1"/>
+    <col min="1" max="1" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -9600,7 +9671,7 @@
         <v>43941</v>
       </c>
       <c r="B42" s="2">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -9704,7 +9775,7 @@
         <v>43954</v>
       </c>
       <c r="B55" s="2">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -9712,7 +9783,7 @@
         <v>43955</v>
       </c>
       <c r="B56" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -9776,7 +9847,7 @@
         <v>43963</v>
       </c>
       <c r="B64" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -9808,7 +9879,7 @@
         <v>43967</v>
       </c>
       <c r="B68" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -9824,7 +9895,7 @@
         <v>43969</v>
       </c>
       <c r="B70" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -9864,7 +9935,7 @@
         <v>43974</v>
       </c>
       <c r="B75" s="2">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -9872,7 +9943,7 @@
         <v>43975</v>
       </c>
       <c r="B76" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -9880,7 +9951,7 @@
         <v>43976</v>
       </c>
       <c r="B77" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -9888,7 +9959,7 @@
         <v>43977</v>
       </c>
       <c r="B78" s="2">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -9896,7 +9967,7 @@
         <v>43978</v>
       </c>
       <c r="B79" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -9904,7 +9975,7 @@
         <v>43979</v>
       </c>
       <c r="B80" s="2">
-        <v>24</v>
+        <v>34</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -9912,7 +9983,7 @@
         <v>43980</v>
       </c>
       <c r="B81" s="2">
-        <v>22</v>
+        <v>32</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -9920,7 +9991,7 @@
         <v>43981</v>
       </c>
       <c r="B82" s="2">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -9928,7 +9999,7 @@
         <v>43982</v>
       </c>
       <c r="B83" s="2">
-        <v>18</v>
+        <v>33</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -9936,7 +10007,7 @@
         <v>43983</v>
       </c>
       <c r="B84" s="2">
-        <v>16</v>
+        <v>27</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -9944,7 +10015,7 @@
         <v>43984</v>
       </c>
       <c r="B85" s="2">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -9952,7 +10023,7 @@
         <v>43985</v>
       </c>
       <c r="B86" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -9960,7 +10031,7 @@
         <v>43986</v>
       </c>
       <c r="B87" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -9968,7 +10039,7 @@
         <v>36</v>
       </c>
       <c r="B88" s="2">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -9978,13 +10049,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B92"/>
+  <dimension ref="A1:B93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="15.08984375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -10351,7 +10425,7 @@
         <v>43940</v>
       </c>
       <c r="B46" s="2">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -10711,7 +10785,7 @@
         <v>43985</v>
       </c>
       <c r="B91" s="2">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -10719,7 +10793,15 @@
         <v>43986</v>
       </c>
       <c r="B92" s="2">
-        <v>2</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="1">
+        <v>43987</v>
+      </c>
+      <c r="B93" s="2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -10732,7 +10814,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -10759,10 +10841,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="2">
-        <v>254</v>
+        <v>264</v>
       </c>
       <c r="C2" s="2">
-        <v>159.14189147949219</v>
+        <v>165.40731811523438</v>
       </c>
       <c r="D2" s="2">
         <v>4</v>
@@ -10776,10 +10858,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>1264</v>
+        <v>1277</v>
       </c>
       <c r="C3" s="2">
-        <v>438.94070434570313</v>
+        <v>443.45513916015625</v>
       </c>
       <c r="D3" s="2">
         <v>60</v>
@@ -10793,10 +10875,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C4" s="2">
-        <v>145.76283264160156</v>
+        <v>147.43826293945313</v>
       </c>
       <c r="D4" s="2">
         <v>5</v>
@@ -10810,16 +10892,16 @@
         <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>1400</v>
+        <v>1435</v>
       </c>
       <c r="C5" s="2">
-        <v>487.15646362304688</v>
+        <v>499.33538818359375</v>
       </c>
       <c r="D5" s="2">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E5" s="2">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -10827,10 +10909,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="2">
-        <v>843</v>
+        <v>870</v>
       </c>
       <c r="C6" s="2">
-        <v>252.5101318359375</v>
+        <v>260.59762573242188</v>
       </c>
       <c r="D6" s="2">
         <v>30</v>
@@ -10844,10 +10926,10 @@
         <v>28</v>
       </c>
       <c r="B7" s="2">
-        <v>757</v>
+        <v>774</v>
       </c>
       <c r="C7" s="2">
-        <v>578.701904296875</v>
+        <v>591.6978759765625</v>
       </c>
       <c r="D7" s="2">
         <v>15</v>
@@ -10861,16 +10943,16 @@
         <v>8</v>
       </c>
       <c r="B8" s="2">
-        <v>1647</v>
+        <v>1681</v>
       </c>
       <c r="C8" s="2">
-        <v>452.9715576171875</v>
+        <v>462.322509765625</v>
       </c>
       <c r="D8" s="2">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E8" s="2">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -10878,16 +10960,16 @@
         <v>9</v>
       </c>
       <c r="B9" s="2">
-        <v>376</v>
+        <v>390</v>
       </c>
       <c r="C9" s="2">
-        <v>153.19052124023438</v>
+        <v>158.89442443847656</v>
       </c>
       <c r="D9" s="2">
         <v>26</v>
       </c>
       <c r="E9" s="2">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -10895,16 +10977,16 @@
         <v>10</v>
       </c>
       <c r="B10" s="2">
-        <v>886</v>
+        <v>897</v>
       </c>
       <c r="C10" s="2">
-        <v>439.7698974609375</v>
+        <v>445.22979736328125</v>
       </c>
       <c r="D10" s="2">
         <v>17</v>
       </c>
       <c r="E10" s="2">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -10912,10 +10994,10 @@
         <v>11</v>
       </c>
       <c r="B11" s="2">
-        <v>461</v>
+        <v>481</v>
       </c>
       <c r="C11" s="2">
-        <v>184.33143615722656</v>
+        <v>192.32846069335938</v>
       </c>
       <c r="D11" s="2">
         <v>37</v>
@@ -10929,10 +11011,10 @@
         <v>12</v>
       </c>
       <c r="B12" s="2">
-        <v>1892</v>
+        <v>1928</v>
       </c>
       <c r="C12" s="2">
-        <v>137.31767272949219</v>
+        <v>139.93048095703125</v>
       </c>
       <c r="D12" s="2">
         <v>95</v>
@@ -10946,16 +11028,16 @@
         <v>13</v>
       </c>
       <c r="B13" s="2">
-        <v>14108</v>
+        <v>14366</v>
       </c>
       <c r="C13" s="2">
-        <v>593.50103759765625</v>
+        <v>604.35467529296875</v>
       </c>
       <c r="D13" s="2">
-        <v>815</v>
+        <v>818</v>
       </c>
       <c r="E13" s="2">
-        <v>2103</v>
+        <v>2136</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -10963,16 +11045,16 @@
         <v>14</v>
       </c>
       <c r="B14" s="2">
-        <v>1643</v>
+        <v>1655</v>
       </c>
       <c r="C14" s="2">
-        <v>552.19464111328125</v>
+        <v>556.22772216796875</v>
       </c>
       <c r="D14" s="2">
         <v>125</v>
       </c>
       <c r="E14" s="2">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -10980,16 +11062,16 @@
         <v>15</v>
       </c>
       <c r="B15" s="2">
-        <v>2077</v>
+        <v>2136</v>
       </c>
       <c r="C15" s="2">
-        <v>541.28997802734375</v>
+        <v>556.66607666015625</v>
       </c>
       <c r="D15" s="2">
         <v>132</v>
       </c>
       <c r="E15" s="2">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -10997,16 +11079,16 @@
         <v>16</v>
       </c>
       <c r="B16" s="2">
-        <v>582</v>
+        <v>599</v>
       </c>
       <c r="C16" s="2">
-        <v>206.08042907714844</v>
+        <v>212.09996032714844</v>
       </c>
       <c r="D16" s="2">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E16" s="2">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -11014,16 +11096,16 @@
         <v>17</v>
       </c>
       <c r="B17" s="2">
-        <v>513</v>
+        <v>518</v>
       </c>
       <c r="C17" s="2">
-        <v>188.78617858886719</v>
+        <v>190.62619018554688</v>
       </c>
       <c r="D17" s="2">
         <v>28</v>
       </c>
       <c r="E17" s="2">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -11031,10 +11113,10 @@
         <v>18</v>
       </c>
       <c r="B18" s="2">
-        <v>806</v>
+        <v>835</v>
       </c>
       <c r="C18" s="2">
-        <v>328.51431274414063</v>
+        <v>340.33428955078125</v>
       </c>
       <c r="D18" s="2">
         <v>40</v>
@@ -11048,16 +11130,16 @@
         <v>19</v>
       </c>
       <c r="B19" s="2">
-        <v>1401</v>
+        <v>1434</v>
       </c>
       <c r="C19" s="2">
-        <v>507.8939208984375</v>
+        <v>519.857177734375</v>
       </c>
       <c r="D19" s="2">
         <v>44</v>
       </c>
       <c r="E19" s="2">
-        <v>139</v>
+        <v>148</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -11065,16 +11147,16 @@
         <v>29</v>
       </c>
       <c r="B20" s="2">
-        <v>6833</v>
+        <v>7218</v>
       </c>
       <c r="C20" s="2">
-        <v>395.91372680664063</v>
+        <v>418.22119140625</v>
       </c>
       <c r="D20" s="2">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="E20" s="2">
-        <v>582</v>
+        <v>600</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -11082,10 +11164,10 @@
         <v>21</v>
       </c>
       <c r="B21" s="2">
-        <v>1894</v>
+        <v>1896</v>
       </c>
       <c r="C21" s="2">
-        <v>621.380859375</v>
+        <v>622.03704833984375</v>
       </c>
       <c r="D21" s="2">
         <v>73</v>
@@ -11099,10 +11181,10 @@
         <v>22</v>
       </c>
       <c r="B22" s="2">
-        <v>2159</v>
+        <v>2197</v>
       </c>
       <c r="C22" s="2">
-        <v>463.80734252929688</v>
+        <v>471.970703125</v>
       </c>
       <c r="D22" s="2">
         <v>100</v>
@@ -11145,13 +11227,13 @@
         <v>34</v>
       </c>
       <c r="B2" s="2">
-        <v>16631</v>
+        <v>17078</v>
       </c>
       <c r="C2" s="2">
-        <v>1579</v>
+        <v>1586</v>
       </c>
       <c r="D2" s="2">
-        <v>2503</v>
+        <v>2545</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -11159,13 +11241,13 @@
         <v>35</v>
       </c>
       <c r="B3" s="2">
-        <v>25251</v>
+        <v>25860</v>
       </c>
       <c r="C3" s="2">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="D3" s="2">
-        <v>2059</v>
+        <v>2094</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -11191,8 +11273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -11216,7 +11298,7 @@
         <v>38</v>
       </c>
       <c r="B2" s="2">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="C2" s="2">
         <v>5</v>
@@ -11230,7 +11312,7 @@
         <v>39</v>
       </c>
       <c r="B3" s="2">
-        <v>518</v>
+        <v>557</v>
       </c>
       <c r="C3" s="2">
         <v>9</v>
@@ -11244,10 +11326,10 @@
         <v>40</v>
       </c>
       <c r="B4" s="2">
-        <v>4058</v>
+        <v>4207</v>
       </c>
       <c r="C4" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D4" s="2">
         <v>8</v>
@@ -11258,7 +11340,7 @@
         <v>41</v>
       </c>
       <c r="B5" s="2">
-        <v>5433</v>
+        <v>5634</v>
       </c>
       <c r="C5" s="2">
         <v>95</v>
@@ -11272,10 +11354,10 @@
         <v>42</v>
       </c>
       <c r="B6" s="2">
-        <v>6463</v>
+        <v>6658</v>
       </c>
       <c r="C6" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D6" s="2">
         <v>42</v>
@@ -11286,13 +11368,13 @@
         <v>43</v>
       </c>
       <c r="B7" s="2">
-        <v>7705</v>
+        <v>7922</v>
       </c>
       <c r="C7" s="2">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="D7" s="2">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -11300,13 +11382,13 @@
         <v>44</v>
       </c>
       <c r="B8" s="2">
-        <v>5020</v>
+        <v>5117</v>
       </c>
       <c r="C8" s="2">
-        <v>643</v>
+        <v>648</v>
       </c>
       <c r="D8" s="2">
-        <v>324</v>
+        <v>336</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -11314,13 +11396,13 @@
         <v>45</v>
       </c>
       <c r="B9" s="2">
-        <v>4288</v>
+        <v>4350</v>
       </c>
       <c r="C9" s="2">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="D9" s="2">
-        <v>1002</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -11328,13 +11410,13 @@
         <v>46</v>
       </c>
       <c r="B10" s="2">
-        <v>5284</v>
+        <v>5347</v>
       </c>
       <c r="C10" s="2">
         <v>85</v>
       </c>
       <c r="D10" s="2">
-        <v>1874</v>
+        <v>1906</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -11342,13 +11424,13 @@
         <v>47</v>
       </c>
       <c r="B11" s="2">
-        <v>2903</v>
+        <v>2930</v>
       </c>
       <c r="C11" s="2">
         <v>1</v>
       </c>
       <c r="D11" s="2">
-        <v>1165</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -11356,7 +11438,7 @@
         <v>36</v>
       </c>
       <c r="B12" s="2">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" s="2">
         <v>0</v>
@@ -11374,7 +11456,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-05 12:09) (#83)
Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/output/snapshot/9c24c2d6-bc87-568a-aff3-c42f38603962.xlsx
+++ b/output/snapshot/9c24c2d6-bc87-568a-aff3-c42f38603962.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Antal per dag region" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Totalt antal per region" sheetId="4" r:id="rId4"/>
     <sheet name="Totalt antal per kön" sheetId="5" r:id="rId5"/>
     <sheet name="Totalt antal per åldersgrupp" sheetId="6" r:id="rId6"/>
-    <sheet name="FOHM  4 Jun 2020" sheetId="7" r:id="rId7"/>
+    <sheet name="FOHM  5 Jun 2020" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -505,15 +505,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W123"/>
+  <dimension ref="A1:W124"/>
   <sheetViews>
-    <sheetView topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="B102" sqref="B1:B1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.54296875" customWidth="1"/>
+    <col min="1" max="1" width="12.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
@@ -3929,7 +3929,7 @@
         <v>43912</v>
       </c>
       <c r="B49" s="2">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C49" s="2">
         <v>0</v>
@@ -3959,7 +3959,7 @@
         <v>0</v>
       </c>
       <c r="L49" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M49" s="2">
         <v>3</v>
@@ -5562,7 +5562,7 @@
         <v>43935</v>
       </c>
       <c r="B72" s="2">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C72" s="2">
         <v>1</v>
@@ -5583,7 +5583,7 @@
         <v>14</v>
       </c>
       <c r="I72" s="2">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J72" s="2">
         <v>5</v>
@@ -8598,10 +8598,10 @@
         <v>41</v>
       </c>
       <c r="T114" s="2">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="U114" s="2">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="V114" s="2">
         <v>28</v>
@@ -8713,13 +8713,13 @@
         <v>18</v>
       </c>
       <c r="K116" s="2">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L116" s="2">
         <v>6</v>
       </c>
       <c r="M116" s="2">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N116" s="2">
         <v>282</v>
@@ -9112,7 +9112,7 @@
         <v>43985</v>
       </c>
       <c r="B122" s="2">
-        <v>1044</v>
+        <v>1070</v>
       </c>
       <c r="C122" s="2">
         <v>18</v>
@@ -9124,7 +9124,7 @@
         <v>1</v>
       </c>
       <c r="F122" s="2">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G122" s="2">
         <v>11</v>
@@ -9148,10 +9148,10 @@
         <v>38</v>
       </c>
       <c r="N122" s="2">
-        <v>234</v>
+        <v>250</v>
       </c>
       <c r="O122" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P122" s="2">
         <v>50</v>
@@ -9163,13 +9163,13 @@
         <v>5</v>
       </c>
       <c r="S122" s="2">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="T122" s="2">
         <v>33</v>
       </c>
       <c r="U122" s="2">
-        <v>421</v>
+        <v>429</v>
       </c>
       <c r="V122" s="2">
         <v>24</v>
@@ -9183,70 +9183,141 @@
         <v>43986</v>
       </c>
       <c r="B123" s="2">
-        <v>194</v>
+        <v>997</v>
       </c>
       <c r="C123" s="2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D123" s="2">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E123" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F123" s="2">
+        <v>44</v>
+      </c>
+      <c r="G123" s="2">
+        <v>22</v>
+      </c>
+      <c r="H123" s="2">
+        <v>15</v>
+      </c>
+      <c r="I123" s="2">
+        <v>26</v>
+      </c>
+      <c r="J123" s="2">
+        <v>14</v>
+      </c>
+      <c r="K123" s="2">
+        <v>11</v>
+      </c>
+      <c r="L123" s="2">
+        <v>19</v>
+      </c>
+      <c r="M123" s="2">
+        <v>42</v>
+      </c>
+      <c r="N123" s="2">
+        <v>219</v>
+      </c>
+      <c r="O123" s="2">
+        <v>12</v>
+      </c>
+      <c r="P123" s="2">
+        <v>57</v>
+      </c>
+      <c r="Q123" s="2">
+        <v>21</v>
+      </c>
+      <c r="R123" s="2">
+        <v>5</v>
+      </c>
+      <c r="S123" s="2">
+        <v>25</v>
+      </c>
+      <c r="T123" s="2">
+        <v>33</v>
+      </c>
+      <c r="U123" s="2">
+        <v>363</v>
+      </c>
+      <c r="V123" s="2">
+        <v>8</v>
+      </c>
+      <c r="W123" s="2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="124" spans="1:23">
+      <c r="A124" s="1">
+        <v>43987</v>
+      </c>
+      <c r="B124" s="2">
+        <v>227</v>
+      </c>
+      <c r="C124" s="2">
+        <v>0</v>
+      </c>
+      <c r="D124" s="2">
+        <v>0</v>
+      </c>
+      <c r="E124" s="2">
+        <v>0</v>
+      </c>
+      <c r="F124" s="2">
+        <v>9</v>
+      </c>
+      <c r="G124" s="2">
+        <v>5</v>
+      </c>
+      <c r="H124" s="2">
+        <v>6</v>
+      </c>
+      <c r="I124" s="2">
+        <v>13</v>
+      </c>
+      <c r="J124" s="2">
+        <v>0</v>
+      </c>
+      <c r="K124" s="2">
+        <v>0</v>
+      </c>
+      <c r="L124" s="2">
+        <v>1</v>
+      </c>
+      <c r="M124" s="2">
+        <v>6</v>
+      </c>
+      <c r="N124" s="2">
+        <v>56</v>
+      </c>
+      <c r="O124" s="2">
+        <v>1</v>
+      </c>
+      <c r="P124" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q124" s="2">
+        <v>4</v>
+      </c>
+      <c r="R124" s="2">
+        <v>0</v>
+      </c>
+      <c r="S124" s="2">
+        <v>6</v>
+      </c>
+      <c r="T124" s="2">
         <v>17</v>
       </c>
-      <c r="G123" s="2">
-        <v>0</v>
-      </c>
-      <c r="H123" s="2">
-        <v>4</v>
-      </c>
-      <c r="I123" s="2">
-        <v>4</v>
-      </c>
-      <c r="J123" s="2">
-        <v>0</v>
-      </c>
-      <c r="K123" s="2">
-        <v>1</v>
-      </c>
-      <c r="L123" s="2">
-        <v>1</v>
-      </c>
-      <c r="M123" s="2">
-        <v>11</v>
-      </c>
-      <c r="N123" s="2">
-        <v>33</v>
-      </c>
-      <c r="O123" s="2">
-        <v>2</v>
-      </c>
-      <c r="P123" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q123" s="2">
-        <v>8</v>
-      </c>
-      <c r="R123" s="2">
-        <v>0</v>
-      </c>
-      <c r="S123" s="2">
-        <v>4</v>
-      </c>
-      <c r="T123" s="2">
-        <v>16</v>
-      </c>
-      <c r="U123" s="2">
-        <v>58</v>
-      </c>
-      <c r="V123" s="2">
-        <v>6</v>
-      </c>
-      <c r="W123" s="2">
-        <v>29</v>
+      <c r="U124" s="2">
+        <v>71</v>
+      </c>
+      <c r="V124" s="2">
+        <v>0</v>
+      </c>
+      <c r="W124" s="2">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -9258,13 +9329,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B88"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="A88" sqref="A88"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="B85" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="12.26953125" customWidth="1"/>
+    <col min="1" max="1" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -9600,7 +9671,7 @@
         <v>43941</v>
       </c>
       <c r="B42" s="2">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -9704,7 +9775,7 @@
         <v>43954</v>
       </c>
       <c r="B55" s="2">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -9712,7 +9783,7 @@
         <v>43955</v>
       </c>
       <c r="B56" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -9776,7 +9847,7 @@
         <v>43963</v>
       </c>
       <c r="B64" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -9808,7 +9879,7 @@
         <v>43967</v>
       </c>
       <c r="B68" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -9824,7 +9895,7 @@
         <v>43969</v>
       </c>
       <c r="B70" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -9864,7 +9935,7 @@
         <v>43974</v>
       </c>
       <c r="B75" s="2">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -9872,7 +9943,7 @@
         <v>43975</v>
       </c>
       <c r="B76" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -9880,7 +9951,7 @@
         <v>43976</v>
       </c>
       <c r="B77" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -9888,7 +9959,7 @@
         <v>43977</v>
       </c>
       <c r="B78" s="2">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -9896,7 +9967,7 @@
         <v>43978</v>
       </c>
       <c r="B79" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -9904,7 +9975,7 @@
         <v>43979</v>
       </c>
       <c r="B80" s="2">
-        <v>24</v>
+        <v>34</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -9912,7 +9983,7 @@
         <v>43980</v>
       </c>
       <c r="B81" s="2">
-        <v>22</v>
+        <v>32</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -9920,7 +9991,7 @@
         <v>43981</v>
       </c>
       <c r="B82" s="2">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -9928,7 +9999,7 @@
         <v>43982</v>
       </c>
       <c r="B83" s="2">
-        <v>18</v>
+        <v>33</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -9936,7 +10007,7 @@
         <v>43983</v>
       </c>
       <c r="B84" s="2">
-        <v>16</v>
+        <v>27</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -9944,7 +10015,7 @@
         <v>43984</v>
       </c>
       <c r="B85" s="2">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -9952,7 +10023,7 @@
         <v>43985</v>
       </c>
       <c r="B86" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -9960,7 +10031,7 @@
         <v>43986</v>
       </c>
       <c r="B87" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -9968,7 +10039,7 @@
         <v>36</v>
       </c>
       <c r="B88" s="2">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -9978,13 +10049,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B92"/>
+  <dimension ref="A1:B93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="15.08984375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -10351,7 +10425,7 @@
         <v>43940</v>
       </c>
       <c r="B46" s="2">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -10711,7 +10785,7 @@
         <v>43985</v>
       </c>
       <c r="B91" s="2">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -10719,7 +10793,15 @@
         <v>43986</v>
       </c>
       <c r="B92" s="2">
-        <v>2</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="1">
+        <v>43987</v>
+      </c>
+      <c r="B93" s="2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -10732,7 +10814,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -10759,10 +10841,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="2">
-        <v>254</v>
+        <v>264</v>
       </c>
       <c r="C2" s="2">
-        <v>159.14189147949219</v>
+        <v>165.40731811523438</v>
       </c>
       <c r="D2" s="2">
         <v>4</v>
@@ -10776,10 +10858,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>1264</v>
+        <v>1277</v>
       </c>
       <c r="C3" s="2">
-        <v>438.94070434570313</v>
+        <v>443.45513916015625</v>
       </c>
       <c r="D3" s="2">
         <v>60</v>
@@ -10793,10 +10875,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C4" s="2">
-        <v>145.76283264160156</v>
+        <v>147.43826293945313</v>
       </c>
       <c r="D4" s="2">
         <v>5</v>
@@ -10810,16 +10892,16 @@
         <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>1400</v>
+        <v>1435</v>
       </c>
       <c r="C5" s="2">
-        <v>487.15646362304688</v>
+        <v>499.33538818359375</v>
       </c>
       <c r="D5" s="2">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E5" s="2">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -10827,10 +10909,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="2">
-        <v>843</v>
+        <v>870</v>
       </c>
       <c r="C6" s="2">
-        <v>252.5101318359375</v>
+        <v>260.59762573242188</v>
       </c>
       <c r="D6" s="2">
         <v>30</v>
@@ -10844,10 +10926,10 @@
         <v>28</v>
       </c>
       <c r="B7" s="2">
-        <v>757</v>
+        <v>774</v>
       </c>
       <c r="C7" s="2">
-        <v>578.701904296875</v>
+        <v>591.6978759765625</v>
       </c>
       <c r="D7" s="2">
         <v>15</v>
@@ -10861,16 +10943,16 @@
         <v>8</v>
       </c>
       <c r="B8" s="2">
-        <v>1647</v>
+        <v>1681</v>
       </c>
       <c r="C8" s="2">
-        <v>452.9715576171875</v>
+        <v>462.322509765625</v>
       </c>
       <c r="D8" s="2">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E8" s="2">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -10878,16 +10960,16 @@
         <v>9</v>
       </c>
       <c r="B9" s="2">
-        <v>376</v>
+        <v>390</v>
       </c>
       <c r="C9" s="2">
-        <v>153.19052124023438</v>
+        <v>158.89442443847656</v>
       </c>
       <c r="D9" s="2">
         <v>26</v>
       </c>
       <c r="E9" s="2">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -10895,16 +10977,16 @@
         <v>10</v>
       </c>
       <c r="B10" s="2">
-        <v>886</v>
+        <v>897</v>
       </c>
       <c r="C10" s="2">
-        <v>439.7698974609375</v>
+        <v>445.22979736328125</v>
       </c>
       <c r="D10" s="2">
         <v>17</v>
       </c>
       <c r="E10" s="2">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -10912,10 +10994,10 @@
         <v>11</v>
       </c>
       <c r="B11" s="2">
-        <v>461</v>
+        <v>481</v>
       </c>
       <c r="C11" s="2">
-        <v>184.33143615722656</v>
+        <v>192.32846069335938</v>
       </c>
       <c r="D11" s="2">
         <v>37</v>
@@ -10929,10 +11011,10 @@
         <v>12</v>
       </c>
       <c r="B12" s="2">
-        <v>1892</v>
+        <v>1928</v>
       </c>
       <c r="C12" s="2">
-        <v>137.31767272949219</v>
+        <v>139.93048095703125</v>
       </c>
       <c r="D12" s="2">
         <v>95</v>
@@ -10946,16 +11028,16 @@
         <v>13</v>
       </c>
       <c r="B13" s="2">
-        <v>14108</v>
+        <v>14366</v>
       </c>
       <c r="C13" s="2">
-        <v>593.50103759765625</v>
+        <v>604.35467529296875</v>
       </c>
       <c r="D13" s="2">
-        <v>815</v>
+        <v>818</v>
       </c>
       <c r="E13" s="2">
-        <v>2103</v>
+        <v>2136</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -10963,16 +11045,16 @@
         <v>14</v>
       </c>
       <c r="B14" s="2">
-        <v>1643</v>
+        <v>1655</v>
       </c>
       <c r="C14" s="2">
-        <v>552.19464111328125</v>
+        <v>556.22772216796875</v>
       </c>
       <c r="D14" s="2">
         <v>125</v>
       </c>
       <c r="E14" s="2">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -10980,16 +11062,16 @@
         <v>15</v>
       </c>
       <c r="B15" s="2">
-        <v>2077</v>
+        <v>2136</v>
       </c>
       <c r="C15" s="2">
-        <v>541.28997802734375</v>
+        <v>556.66607666015625</v>
       </c>
       <c r="D15" s="2">
         <v>132</v>
       </c>
       <c r="E15" s="2">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -10997,16 +11079,16 @@
         <v>16</v>
       </c>
       <c r="B16" s="2">
-        <v>582</v>
+        <v>599</v>
       </c>
       <c r="C16" s="2">
-        <v>206.08042907714844</v>
+        <v>212.09996032714844</v>
       </c>
       <c r="D16" s="2">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E16" s="2">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -11014,16 +11096,16 @@
         <v>17</v>
       </c>
       <c r="B17" s="2">
-        <v>513</v>
+        <v>518</v>
       </c>
       <c r="C17" s="2">
-        <v>188.78617858886719</v>
+        <v>190.62619018554688</v>
       </c>
       <c r="D17" s="2">
         <v>28</v>
       </c>
       <c r="E17" s="2">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -11031,10 +11113,10 @@
         <v>18</v>
       </c>
       <c r="B18" s="2">
-        <v>806</v>
+        <v>835</v>
       </c>
       <c r="C18" s="2">
-        <v>328.51431274414063</v>
+        <v>340.33428955078125</v>
       </c>
       <c r="D18" s="2">
         <v>40</v>
@@ -11048,16 +11130,16 @@
         <v>19</v>
       </c>
       <c r="B19" s="2">
-        <v>1401</v>
+        <v>1434</v>
       </c>
       <c r="C19" s="2">
-        <v>507.8939208984375</v>
+        <v>519.857177734375</v>
       </c>
       <c r="D19" s="2">
         <v>44</v>
       </c>
       <c r="E19" s="2">
-        <v>139</v>
+        <v>148</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -11065,16 +11147,16 @@
         <v>29</v>
       </c>
       <c r="B20" s="2">
-        <v>6833</v>
+        <v>7218</v>
       </c>
       <c r="C20" s="2">
-        <v>395.91372680664063</v>
+        <v>418.22119140625</v>
       </c>
       <c r="D20" s="2">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="E20" s="2">
-        <v>582</v>
+        <v>600</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -11082,10 +11164,10 @@
         <v>21</v>
       </c>
       <c r="B21" s="2">
-        <v>1894</v>
+        <v>1896</v>
       </c>
       <c r="C21" s="2">
-        <v>621.380859375</v>
+        <v>622.03704833984375</v>
       </c>
       <c r="D21" s="2">
         <v>73</v>
@@ -11099,10 +11181,10 @@
         <v>22</v>
       </c>
       <c r="B22" s="2">
-        <v>2159</v>
+        <v>2197</v>
       </c>
       <c r="C22" s="2">
-        <v>463.80734252929688</v>
+        <v>471.970703125</v>
       </c>
       <c r="D22" s="2">
         <v>100</v>
@@ -11145,13 +11227,13 @@
         <v>34</v>
       </c>
       <c r="B2" s="2">
-        <v>16631</v>
+        <v>17078</v>
       </c>
       <c r="C2" s="2">
-        <v>1579</v>
+        <v>1586</v>
       </c>
       <c r="D2" s="2">
-        <v>2503</v>
+        <v>2545</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -11159,13 +11241,13 @@
         <v>35</v>
       </c>
       <c r="B3" s="2">
-        <v>25251</v>
+        <v>25860</v>
       </c>
       <c r="C3" s="2">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="D3" s="2">
-        <v>2059</v>
+        <v>2094</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -11191,8 +11273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -11216,7 +11298,7 @@
         <v>38</v>
       </c>
       <c r="B2" s="2">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="C2" s="2">
         <v>5</v>
@@ -11230,7 +11312,7 @@
         <v>39</v>
       </c>
       <c r="B3" s="2">
-        <v>518</v>
+        <v>557</v>
       </c>
       <c r="C3" s="2">
         <v>9</v>
@@ -11244,10 +11326,10 @@
         <v>40</v>
       </c>
       <c r="B4" s="2">
-        <v>4058</v>
+        <v>4207</v>
       </c>
       <c r="C4" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D4" s="2">
         <v>8</v>
@@ -11258,7 +11340,7 @@
         <v>41</v>
       </c>
       <c r="B5" s="2">
-        <v>5433</v>
+        <v>5634</v>
       </c>
       <c r="C5" s="2">
         <v>95</v>
@@ -11272,10 +11354,10 @@
         <v>42</v>
       </c>
       <c r="B6" s="2">
-        <v>6463</v>
+        <v>6658</v>
       </c>
       <c r="C6" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D6" s="2">
         <v>42</v>
@@ -11286,13 +11368,13 @@
         <v>43</v>
       </c>
       <c r="B7" s="2">
-        <v>7705</v>
+        <v>7922</v>
       </c>
       <c r="C7" s="2">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="D7" s="2">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -11300,13 +11382,13 @@
         <v>44</v>
       </c>
       <c r="B8" s="2">
-        <v>5020</v>
+        <v>5117</v>
       </c>
       <c r="C8" s="2">
-        <v>643</v>
+        <v>648</v>
       </c>
       <c r="D8" s="2">
-        <v>324</v>
+        <v>336</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -11314,13 +11396,13 @@
         <v>45</v>
       </c>
       <c r="B9" s="2">
-        <v>4288</v>
+        <v>4350</v>
       </c>
       <c r="C9" s="2">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="D9" s="2">
-        <v>1002</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -11328,13 +11410,13 @@
         <v>46</v>
       </c>
       <c r="B10" s="2">
-        <v>5284</v>
+        <v>5347</v>
       </c>
       <c r="C10" s="2">
         <v>85</v>
       </c>
       <c r="D10" s="2">
-        <v>1874</v>
+        <v>1906</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -11342,13 +11424,13 @@
         <v>47</v>
       </c>
       <c r="B11" s="2">
-        <v>2903</v>
+        <v>2930</v>
       </c>
       <c r="C11" s="2">
         <v>1</v>
       </c>
       <c r="D11" s="2">
-        <v>1165</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -11356,7 +11438,7 @@
         <v>36</v>
       </c>
       <c r="B12" s="2">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" s="2">
         <v>0</v>
@@ -11374,7 +11456,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-07 12:09)
</commit_message>
<xml_diff>
--- a/output/snapshot/9c24c2d6-bc87-568a-aff3-c42f38603962.xlsx
+++ b/output/snapshot/9c24c2d6-bc87-568a-aff3-c42f38603962.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Data\covid-19\Do-filer och analys\filer till dashboard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\dfs-srv1.fohm.local\Common\Data\covid-19\Do-filer och analys\filer till dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16050" windowHeight="10110" firstSheet="4" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Antal per dag region" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,14 @@
     <sheet name="Totalt antal per region" sheetId="4" r:id="rId4"/>
     <sheet name="Totalt antal per kön" sheetId="5" r:id="rId5"/>
     <sheet name="Totalt antal per åldersgrupp" sheetId="6" r:id="rId6"/>
-    <sheet name="FOHM  6 Jun 2020" sheetId="7" r:id="rId7"/>
+    <sheet name="FOHM  7 Jun 2020" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="50">
   <si>
     <t>Statistikdatum</t>
   </si>
@@ -175,9 +175,6 @@
   </si>
   <si>
     <t>Data uppdateras dagligen kl 11.30 och finns tillgängliga dagligen kl 14.00. Läs mer på https://www.folkhalsomyndigheten.se/smittskydd-beredskap/utbrott/aktuella-utbrott/covid-19/aktuellt-epidemiologiskt-lage/</t>
-  </si>
-  <si>
-    <t>Uppgift saknaa</t>
   </si>
 </sst>
 </file>
@@ -508,11 +505,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W125"/>
+  <dimension ref="A1:W126"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:23">
       <c r="A1" t="s">
@@ -9252,7 +9252,7 @@
         <v>43987</v>
       </c>
       <c r="B124" s="2">
-        <v>1016</v>
+        <v>1140</v>
       </c>
       <c r="C124" s="2">
         <v>10</v>
@@ -9267,7 +9267,7 @@
         <v>43</v>
       </c>
       <c r="G124" s="2">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H124" s="2">
         <v>13</v>
@@ -9282,13 +9282,13 @@
         <v>19</v>
       </c>
       <c r="L124" s="2">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M124" s="2">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="N124" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="O124" s="2">
         <v>3</v>
@@ -9297,19 +9297,19 @@
         <v>34</v>
       </c>
       <c r="Q124" s="2">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="R124" s="2">
         <v>5</v>
       </c>
       <c r="S124" s="2">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="T124" s="2">
         <v>19</v>
       </c>
       <c r="U124" s="2">
-        <v>373</v>
+        <v>483</v>
       </c>
       <c r="V124" s="2">
         <v>46</v>
@@ -9323,70 +9323,141 @@
         <v>43988</v>
       </c>
       <c r="B125" s="2">
-        <v>114</v>
+        <v>752</v>
       </c>
       <c r="C125" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D125" s="2">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E125" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F125" s="2">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="G125" s="2">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="H125" s="2">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="I125" s="2">
+        <v>40</v>
+      </c>
+      <c r="J125" s="2">
+        <v>1</v>
+      </c>
+      <c r="K125" s="2">
+        <v>0</v>
+      </c>
+      <c r="L125" s="2">
+        <v>7</v>
+      </c>
+      <c r="M125" s="2">
+        <v>23</v>
+      </c>
+      <c r="N125" s="2">
+        <v>188</v>
+      </c>
+      <c r="O125" s="2">
+        <v>1</v>
+      </c>
+      <c r="P125" s="2">
+        <v>42</v>
+      </c>
+      <c r="Q125" s="2">
+        <v>24</v>
+      </c>
+      <c r="R125" s="2">
+        <v>8</v>
+      </c>
+      <c r="S125" s="2">
+        <v>7</v>
+      </c>
+      <c r="T125" s="2">
+        <v>0</v>
+      </c>
+      <c r="U125" s="2">
+        <v>257</v>
+      </c>
+      <c r="V125" s="2">
+        <v>15</v>
+      </c>
+      <c r="W125" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="126" spans="1:23">
+      <c r="A126" s="1">
+        <v>43989</v>
+      </c>
+      <c r="B126" s="2">
+        <v>81</v>
+      </c>
+      <c r="C126" s="2">
+        <v>0</v>
+      </c>
+      <c r="D126" s="2">
+        <v>1</v>
+      </c>
+      <c r="E126" s="2">
+        <v>0</v>
+      </c>
+      <c r="F126" s="2">
+        <v>2</v>
+      </c>
+      <c r="G126" s="2">
+        <v>6</v>
+      </c>
+      <c r="H126" s="2">
+        <v>0</v>
+      </c>
+      <c r="I126" s="2">
+        <v>0</v>
+      </c>
+      <c r="J126" s="2">
+        <v>1</v>
+      </c>
+      <c r="K126" s="2">
+        <v>0</v>
+      </c>
+      <c r="L126" s="2">
+        <v>0</v>
+      </c>
+      <c r="M126" s="2">
+        <v>2</v>
+      </c>
+      <c r="N126" s="2">
+        <v>12</v>
+      </c>
+      <c r="O126" s="2">
+        <v>0</v>
+      </c>
+      <c r="P126" s="2">
         <v>9</v>
       </c>
-      <c r="J125" s="2">
-        <v>1</v>
-      </c>
-      <c r="K125" s="2">
-        <v>0</v>
-      </c>
-      <c r="L125" s="2">
-        <v>1</v>
-      </c>
-      <c r="M125" s="2">
-        <v>1</v>
-      </c>
-      <c r="N125" s="2">
-        <v>27</v>
-      </c>
-      <c r="O125" s="2">
-        <v>0</v>
-      </c>
-      <c r="P125" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q125" s="2">
-        <v>3</v>
-      </c>
-      <c r="R125" s="2">
-        <v>0</v>
-      </c>
-      <c r="S125" s="2">
-        <v>1</v>
-      </c>
-      <c r="T125" s="2">
-        <v>0</v>
-      </c>
-      <c r="U125" s="2">
-        <v>27</v>
-      </c>
-      <c r="V125" s="2">
-        <v>0</v>
-      </c>
-      <c r="W125" s="2">
-        <v>30</v>
+      <c r="Q126" s="2">
+        <v>2</v>
+      </c>
+      <c r="R126" s="2">
+        <v>1</v>
+      </c>
+      <c r="S126" s="2">
+        <v>0</v>
+      </c>
+      <c r="T126" s="2">
+        <v>0</v>
+      </c>
+      <c r="U126" s="2">
+        <v>44</v>
+      </c>
+      <c r="V126" s="2">
+        <v>0</v>
+      </c>
+      <c r="W126" s="2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -9396,10 +9467,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B89"/>
+  <dimension ref="A1:B90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="B89" sqref="B89"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10049,7 +10120,7 @@
         <v>43980</v>
       </c>
       <c r="B81" s="2">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -10097,7 +10168,7 @@
         <v>43986</v>
       </c>
       <c r="B87" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -10109,10 +10180,16 @@
       </c>
     </row>
     <row r="89" spans="1:2">
-      <c r="A89" s="1" t="s">
-        <v>50</v>
+      <c r="A89" s="1">
+        <v>43988</v>
       </c>
       <c r="B89" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" s="1"/>
+      <c r="B90" s="2">
         <v>10</v>
       </c>
     </row>
@@ -10123,9 +10200,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B93"/>
+  <dimension ref="A1:B95"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -10870,7 +10949,23 @@
         <v>43987</v>
       </c>
       <c r="B93" s="2">
-        <v>4</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" s="1">
+        <v>43988</v>
+      </c>
+      <c r="B94" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" s="1">
+        <v>43989</v>
+      </c>
+      <c r="B95" s="2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -10882,9 +10977,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -10908,10 +11008,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="2">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="C2" s="2">
-        <v>171.67274475097656</v>
+        <v>174.80546569824219</v>
       </c>
       <c r="D2" s="2">
         <v>4</v>
@@ -10925,10 +11025,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>1297</v>
+        <v>1314</v>
       </c>
       <c r="C3" s="2">
-        <v>450.400390625</v>
+        <v>456.30386352539063</v>
       </c>
       <c r="D3" s="2">
         <v>61</v>
@@ -10942,10 +11042,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C4" s="2">
-        <v>149.11369323730469</v>
+        <v>150.78912353515625</v>
       </c>
       <c r="D4" s="2">
         <v>5</v>
@@ -10959,13 +11059,13 @@
         <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>1470</v>
+        <v>1503</v>
       </c>
       <c r="C5" s="2">
-        <v>511.5142822265625</v>
+        <v>522.99725341796875</v>
       </c>
       <c r="D5" s="2">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E5" s="2">
         <v>112</v>
@@ -10976,10 +11076,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="2">
-        <v>887</v>
+        <v>913</v>
       </c>
       <c r="C6" s="2">
-        <v>265.68978881835938</v>
+        <v>273.47775268554688</v>
       </c>
       <c r="D6" s="2">
         <v>31</v>
@@ -10993,16 +11093,16 @@
         <v>28</v>
       </c>
       <c r="B7" s="2">
-        <v>792</v>
+        <v>803</v>
       </c>
       <c r="C7" s="2">
-        <v>605.45831298828125</v>
+        <v>613.867431640625</v>
       </c>
       <c r="D7" s="2">
         <v>15</v>
       </c>
       <c r="E7" s="2">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -11010,13 +11110,13 @@
         <v>8</v>
       </c>
       <c r="B8" s="2">
-        <v>1719</v>
+        <v>1750</v>
       </c>
       <c r="C8" s="2">
-        <v>472.77359008789063</v>
+        <v>481.2994384765625</v>
       </c>
       <c r="D8" s="2">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E8" s="2">
         <v>144</v>
@@ -11027,10 +11127,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C9" s="2">
-        <v>165.0057373046875</v>
+        <v>165.41316223144531</v>
       </c>
       <c r="D9" s="2">
         <v>26</v>
@@ -11061,10 +11161,10 @@
         <v>11</v>
       </c>
       <c r="B11" s="2">
-        <v>495</v>
+        <v>503</v>
       </c>
       <c r="C11" s="2">
-        <v>197.92637634277344</v>
+        <v>201.12518310546875</v>
       </c>
       <c r="D11" s="2">
         <v>37</v>
@@ -11078,10 +11178,10 @@
         <v>12</v>
       </c>
       <c r="B12" s="2">
-        <v>1957</v>
+        <v>1985</v>
       </c>
       <c r="C12" s="2">
-        <v>142.03524780273438</v>
+        <v>144.06742858886719</v>
       </c>
       <c r="D12" s="2">
         <v>97</v>
@@ -11095,16 +11195,16 @@
         <v>13</v>
       </c>
       <c r="B13" s="2">
-        <v>14571</v>
+        <v>14745</v>
       </c>
       <c r="C13" s="2">
-        <v>612.97869873046875</v>
+        <v>620.298583984375</v>
       </c>
       <c r="D13" s="2">
-        <v>822</v>
+        <v>826</v>
       </c>
       <c r="E13" s="2">
-        <v>2137</v>
+        <v>2138</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -11112,10 +11212,10 @@
         <v>14</v>
       </c>
       <c r="B14" s="2">
-        <v>1657</v>
+        <v>1658</v>
       </c>
       <c r="C14" s="2">
-        <v>556.89990234375</v>
+        <v>557.23602294921875</v>
       </c>
       <c r="D14" s="2">
         <v>125</v>
@@ -11129,10 +11229,10 @@
         <v>15</v>
       </c>
       <c r="B15" s="2">
-        <v>2171</v>
+        <v>2221</v>
       </c>
       <c r="C15" s="2">
-        <v>565.7874755859375</v>
+        <v>578.8179931640625</v>
       </c>
       <c r="D15" s="2">
         <v>132</v>
@@ -11146,10 +11246,10 @@
         <v>16</v>
       </c>
       <c r="B16" s="2">
-        <v>606</v>
+        <v>633</v>
       </c>
       <c r="C16" s="2">
-        <v>214.57859802246094</v>
+        <v>224.13902282714844</v>
       </c>
       <c r="D16" s="2">
         <v>24</v>
@@ -11163,10 +11263,10 @@
         <v>17</v>
       </c>
       <c r="B17" s="2">
-        <v>523</v>
+        <v>532</v>
       </c>
       <c r="C17" s="2">
-        <v>192.46621704101563</v>
+        <v>195.77825927734375</v>
       </c>
       <c r="D17" s="2">
         <v>28</v>
@@ -11180,16 +11280,16 @@
         <v>18</v>
       </c>
       <c r="B18" s="2">
-        <v>853</v>
+        <v>860</v>
       </c>
       <c r="C18" s="2">
-        <v>347.67083740234375</v>
+        <v>350.52395629882813</v>
       </c>
       <c r="D18" s="2">
         <v>40</v>
       </c>
       <c r="E18" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -11214,13 +11314,13 @@
         <v>29</v>
       </c>
       <c r="B20" s="2">
-        <v>7589</v>
+        <v>7973</v>
       </c>
       <c r="C20" s="2">
-        <v>439.71746826171875</v>
+        <v>461.96694946289063</v>
       </c>
       <c r="D20" s="2">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="E20" s="2">
         <v>602</v>
@@ -11231,10 +11331,10 @@
         <v>21</v>
       </c>
       <c r="B21" s="2">
-        <v>1942</v>
+        <v>1957</v>
       </c>
       <c r="C21" s="2">
-        <v>637.128662109375</v>
+        <v>642.0498046875</v>
       </c>
       <c r="D21" s="2">
         <v>73</v>
@@ -11248,10 +11348,10 @@
         <v>22</v>
       </c>
       <c r="B22" s="2">
-        <v>2238</v>
+        <v>2253</v>
       </c>
       <c r="C22" s="2">
-        <v>480.77853393554688</v>
+        <v>484.00091552734375</v>
       </c>
       <c r="D22" s="2">
         <v>100</v>
@@ -11269,7 +11369,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -11292,13 +11394,13 @@
         <v>34</v>
       </c>
       <c r="B2" s="2">
-        <v>17493</v>
+        <v>17821</v>
       </c>
       <c r="C2" s="2">
-        <v>1595</v>
+        <v>1603</v>
       </c>
       <c r="D2" s="2">
-        <v>2554</v>
+        <v>2556</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -11306,13 +11408,13 @@
         <v>35</v>
       </c>
       <c r="B3" s="2">
-        <v>26393</v>
+        <v>26908</v>
       </c>
       <c r="C3" s="2">
-        <v>567</v>
+        <v>570</v>
       </c>
       <c r="D3" s="2">
-        <v>2102</v>
+        <v>2103</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -11338,7 +11440,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -11361,7 +11465,7 @@
         <v>38</v>
       </c>
       <c r="B2" s="2">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="C2" s="2">
         <v>5</v>
@@ -11375,7 +11479,7 @@
         <v>39</v>
       </c>
       <c r="B3" s="2">
-        <v>580</v>
+        <v>608</v>
       </c>
       <c r="C3" s="2">
         <v>9</v>
@@ -11389,7 +11493,7 @@
         <v>40</v>
       </c>
       <c r="B4" s="2">
-        <v>4343</v>
+        <v>4479</v>
       </c>
       <c r="C4" s="2">
         <v>81</v>
@@ -11403,10 +11507,10 @@
         <v>41</v>
       </c>
       <c r="B5" s="2">
-        <v>5806</v>
+        <v>5963</v>
       </c>
       <c r="C5" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D5" s="2">
         <v>12</v>
@@ -11417,10 +11521,10 @@
         <v>42</v>
       </c>
       <c r="B6" s="2">
-        <v>6852</v>
+        <v>6994</v>
       </c>
       <c r="C6" s="2">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="D6" s="2">
         <v>42</v>
@@ -11431,10 +11535,10 @@
         <v>43</v>
       </c>
       <c r="B7" s="2">
-        <v>8121</v>
+        <v>8313</v>
       </c>
       <c r="C7" s="2">
-        <v>568</v>
+        <v>571</v>
       </c>
       <c r="D7" s="2">
         <v>137</v>
@@ -11445,10 +11549,10 @@
         <v>44</v>
       </c>
       <c r="B8" s="2">
-        <v>5218</v>
+        <v>5308</v>
       </c>
       <c r="C8" s="2">
-        <v>649</v>
+        <v>652</v>
       </c>
       <c r="D8" s="2">
         <v>336</v>
@@ -11459,13 +11563,13 @@
         <v>45</v>
       </c>
       <c r="B9" s="2">
-        <v>4391</v>
+        <v>4431</v>
       </c>
       <c r="C9" s="2">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="D9" s="2">
-        <v>1022</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -11473,13 +11577,13 @@
         <v>46</v>
       </c>
       <c r="B10" s="2">
-        <v>5396</v>
+        <v>5430</v>
       </c>
       <c r="C10" s="2">
         <v>86</v>
       </c>
       <c r="D10" s="2">
-        <v>1914</v>
+        <v>1916</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -11487,7 +11591,7 @@
         <v>47</v>
       </c>
       <c r="B11" s="2">
-        <v>2957</v>
+        <v>2975</v>
       </c>
       <c r="C11" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-09 12:10)
</commit_message>
<xml_diff>
--- a/output/snapshot/9c24c2d6-bc87-568a-aff3-c42f38603962.xlsx
+++ b/output/snapshot/9c24c2d6-bc87-568a-aff3-c42f38603962.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15480" windowHeight="7030" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19350" windowHeight="11470" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Antal per dag region" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Totalt antal per region" sheetId="4" r:id="rId4"/>
     <sheet name="Totalt antal per kön" sheetId="5" r:id="rId5"/>
     <sheet name="Totalt antal per åldersgrupp" sheetId="6" r:id="rId6"/>
-    <sheet name="FOHM  8 Jun 2020" sheetId="7" r:id="rId7"/>
+    <sheet name="FOHM  9 Jun 2020" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -505,15 +505,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W127"/>
+  <dimension ref="A1:W128"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="B33" sqref="B1:B1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="14.1796875" customWidth="1"/>
+    <col min="1" max="1" width="21.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
@@ -8757,7 +8757,7 @@
         <v>43980</v>
       </c>
       <c r="B117" s="2">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="C117" s="2">
         <v>10</v>
@@ -8793,7 +8793,7 @@
         <v>46</v>
       </c>
       <c r="N117" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="O117" s="2">
         <v>4</v>
@@ -9041,7 +9041,7 @@
         <v>43984</v>
       </c>
       <c r="B121" s="2">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="C121" s="2">
         <v>18</v>
@@ -9092,7 +9092,7 @@
         <v>8</v>
       </c>
       <c r="S121" s="2">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="T121" s="2">
         <v>35</v>
@@ -9254,7 +9254,7 @@
         <v>43987</v>
       </c>
       <c r="B124" s="2">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C124" s="2">
         <v>10</v>
@@ -9317,7 +9317,7 @@
         <v>46</v>
       </c>
       <c r="W124" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="125" spans="1:23">
@@ -9325,7 +9325,7 @@
         <v>43988</v>
       </c>
       <c r="B125" s="2">
-        <v>823</v>
+        <v>825</v>
       </c>
       <c r="C125" s="2">
         <v>5</v>
@@ -9334,10 +9334,10 @@
         <v>16</v>
       </c>
       <c r="E125" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F125" s="2">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G125" s="2">
         <v>19</v>
@@ -9361,7 +9361,7 @@
         <v>23</v>
       </c>
       <c r="N125" s="2">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="O125" s="2">
         <v>1</v>
@@ -9388,7 +9388,7 @@
         <v>19</v>
       </c>
       <c r="W125" s="2">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="126" spans="1:23">
@@ -9396,28 +9396,28 @@
         <v>43989</v>
       </c>
       <c r="B126" s="2">
-        <v>344</v>
+        <v>462</v>
       </c>
       <c r="C126" s="2">
         <v>18</v>
       </c>
       <c r="D126" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E126" s="2">
         <v>0</v>
       </c>
       <c r="F126" s="2">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="G126" s="2">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H126" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I126" s="2">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="J126" s="2">
         <v>3</v>
@@ -9432,34 +9432,34 @@
         <v>12</v>
       </c>
       <c r="N126" s="2">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="O126" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P126" s="2">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="Q126" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R126" s="2">
         <v>4</v>
       </c>
       <c r="S126" s="2">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="T126" s="2">
         <v>0</v>
       </c>
       <c r="U126" s="2">
-        <v>170</v>
+        <v>229</v>
       </c>
       <c r="V126" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="W126" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="127" spans="1:23">
@@ -9467,70 +9467,141 @@
         <v>43990</v>
       </c>
       <c r="B127" s="2">
-        <v>68</v>
+        <v>536</v>
       </c>
       <c r="C127" s="2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D127" s="2">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E127" s="2">
         <v>0</v>
       </c>
       <c r="F127" s="2">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="G127" s="2">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="H127" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I127" s="2">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="J127" s="2">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="K127" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L127" s="2">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="M127" s="2">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="N127" s="2">
-        <v>19</v>
+        <v>128</v>
       </c>
       <c r="O127" s="2">
         <v>10</v>
       </c>
       <c r="P127" s="2">
+        <v>12</v>
+      </c>
+      <c r="Q127" s="2">
+        <v>15</v>
+      </c>
+      <c r="R127" s="2">
+        <v>4</v>
+      </c>
+      <c r="S127" s="2">
+        <v>23</v>
+      </c>
+      <c r="T127" s="2">
+        <v>67</v>
+      </c>
+      <c r="U127" s="2">
+        <v>121</v>
+      </c>
+      <c r="V127" s="2">
         <v>7</v>
       </c>
-      <c r="Q127" s="2">
-        <v>0</v>
-      </c>
-      <c r="R127" s="2">
-        <v>0</v>
-      </c>
-      <c r="S127" s="2">
+      <c r="W127" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:23">
+      <c r="A128" s="1">
+        <v>43991</v>
+      </c>
+      <c r="B128" s="2">
+        <v>202</v>
+      </c>
+      <c r="C128" s="2">
+        <v>0</v>
+      </c>
+      <c r="D128" s="2">
+        <v>1</v>
+      </c>
+      <c r="E128" s="2">
+        <v>0</v>
+      </c>
+      <c r="F128" s="2">
+        <v>0</v>
+      </c>
+      <c r="G128" s="2">
+        <v>4</v>
+      </c>
+      <c r="H128" s="2">
         <v>6</v>
       </c>
-      <c r="T127" s="2">
+      <c r="I128" s="2">
+        <v>6</v>
+      </c>
+      <c r="J128" s="2">
+        <v>0</v>
+      </c>
+      <c r="K128" s="2">
+        <v>0</v>
+      </c>
+      <c r="L128" s="2">
+        <v>1</v>
+      </c>
+      <c r="M128" s="2">
+        <v>0</v>
+      </c>
+      <c r="N128" s="2">
+        <v>42</v>
+      </c>
+      <c r="O128" s="2">
+        <v>2</v>
+      </c>
+      <c r="P128" s="2">
+        <v>11</v>
+      </c>
+      <c r="Q128" s="2">
+        <v>5</v>
+      </c>
+      <c r="R128" s="2">
+        <v>0</v>
+      </c>
+      <c r="S128" s="2">
+        <v>1</v>
+      </c>
+      <c r="T128" s="2">
+        <v>24</v>
+      </c>
+      <c r="U128" s="2">
+        <v>78</v>
+      </c>
+      <c r="V128" s="2">
+        <v>0</v>
+      </c>
+      <c r="W128" s="2">
         <v>21</v>
-      </c>
-      <c r="U127" s="2">
-        <v>3</v>
-      </c>
-      <c r="V127" s="2">
-        <v>0</v>
-      </c>
-      <c r="W127" s="2">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -9540,13 +9611,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B91"/>
+  <dimension ref="A1:B93"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="A91" sqref="A91"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="12.90625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -10193,7 +10267,7 @@
         <v>43980</v>
       </c>
       <c r="B81" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -10217,7 +10291,7 @@
         <v>43983</v>
       </c>
       <c r="B84" s="2">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -10233,7 +10307,7 @@
         <v>43985</v>
       </c>
       <c r="B86" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -10249,7 +10323,7 @@
         <v>43987</v>
       </c>
       <c r="B88" s="2">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -10257,7 +10331,7 @@
         <v>43988</v>
       </c>
       <c r="B89" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -10265,15 +10339,31 @@
         <v>43989</v>
       </c>
       <c r="B90" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="91" spans="1:2">
-      <c r="A91" s="1" t="s">
+      <c r="A91" s="1">
+        <v>43990</v>
+      </c>
+      <c r="B91" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" s="1">
+        <v>43991</v>
+      </c>
+      <c r="B92" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B91" s="2">
-        <v>11</v>
+      <c r="B93" s="2">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -10283,13 +10373,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B95"/>
+  <dimension ref="A1:B96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -10392,7 +10485,7 @@
         <v>43907</v>
       </c>
       <c r="B13" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -10472,7 +10565,7 @@
         <v>43917</v>
       </c>
       <c r="B23" s="2">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -10560,7 +10653,7 @@
         <v>43928</v>
       </c>
       <c r="B34" s="2">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -10568,7 +10661,7 @@
         <v>43929</v>
       </c>
       <c r="B35" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -11016,7 +11109,7 @@
         <v>43985</v>
       </c>
       <c r="B91" s="2">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -11024,7 +11117,7 @@
         <v>43986</v>
       </c>
       <c r="B92" s="2">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -11032,7 +11125,7 @@
         <v>43987</v>
       </c>
       <c r="B93" s="2">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -11040,7 +11133,7 @@
         <v>43988</v>
       </c>
       <c r="B94" s="2">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -11048,7 +11141,15 @@
         <v>43989</v>
       </c>
       <c r="B95" s="2">
-        <v>9</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" s="1">
+        <v>43990</v>
+      </c>
+      <c r="B96" s="2">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -11088,16 +11189,16 @@
         <v>2</v>
       </c>
       <c r="B2" s="2">
-        <v>297</v>
+        <v>307</v>
       </c>
       <c r="C2" s="2">
-        <v>186.08323669433594</v>
+        <v>192.34866333007813</v>
       </c>
       <c r="D2" s="2">
         <v>4</v>
       </c>
       <c r="E2" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -11105,10 +11206,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>1315</v>
+        <v>1329</v>
       </c>
       <c r="C3" s="2">
-        <v>456.651123046875</v>
+        <v>461.5128173828125</v>
       </c>
       <c r="D3" s="2">
         <v>61</v>
@@ -11122,10 +11223,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C4" s="2">
-        <v>150.78912353515625</v>
+        <v>152.46456909179688</v>
       </c>
       <c r="D4" s="2">
         <v>5</v>
@@ -11139,16 +11240,16 @@
         <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>1516</v>
+        <v>1542</v>
       </c>
       <c r="C5" s="2">
-        <v>527.5208740234375</v>
+        <v>536.56805419921875</v>
       </c>
       <c r="D5" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E5" s="2">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -11156,13 +11257,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="2">
-        <v>920</v>
+        <v>937</v>
       </c>
       <c r="C6" s="2">
-        <v>275.57452392578125</v>
+        <v>280.66665649414063</v>
       </c>
       <c r="D6" s="2">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E6" s="2">
         <v>57</v>
@@ -11173,10 +11274,10 @@
         <v>28</v>
       </c>
       <c r="B7" s="2">
-        <v>809</v>
+        <v>817</v>
       </c>
       <c r="C7" s="2">
-        <v>618.4542236328125</v>
+        <v>624.57000732421875</v>
       </c>
       <c r="D7" s="2">
         <v>16</v>
@@ -11190,16 +11291,16 @@
         <v>8</v>
       </c>
       <c r="B8" s="2">
-        <v>1751</v>
+        <v>1792</v>
       </c>
       <c r="C8" s="2">
-        <v>481.57449340820313</v>
+        <v>492.85064697265625</v>
       </c>
       <c r="D8" s="2">
         <v>78</v>
       </c>
       <c r="E8" s="2">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -11207,16 +11308,16 @@
         <v>9</v>
       </c>
       <c r="B9" s="2">
-        <v>408</v>
+        <v>421</v>
       </c>
       <c r="C9" s="2">
-        <v>166.22801208496094</v>
+        <v>171.52449035644531</v>
       </c>
       <c r="D9" s="2">
         <v>27</v>
       </c>
       <c r="E9" s="2">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -11224,16 +11325,16 @@
         <v>10</v>
       </c>
       <c r="B10" s="2">
-        <v>930</v>
+        <v>935</v>
       </c>
       <c r="C10" s="2">
-        <v>461.60946655273438</v>
+        <v>464.09124755859375</v>
       </c>
       <c r="D10" s="2">
         <v>17</v>
       </c>
       <c r="E10" s="2">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -11241,16 +11342,16 @@
         <v>11</v>
       </c>
       <c r="B11" s="2">
-        <v>503</v>
+        <v>533</v>
       </c>
       <c r="C11" s="2">
-        <v>201.12518310546875</v>
+        <v>213.12071228027344</v>
       </c>
       <c r="D11" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E11" s="2">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -11258,16 +11359,16 @@
         <v>12</v>
       </c>
       <c r="B12" s="2">
-        <v>1995</v>
+        <v>2028</v>
       </c>
       <c r="C12" s="2">
-        <v>144.793212890625</v>
+        <v>147.18829345703125</v>
       </c>
       <c r="D12" s="2">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="E12" s="2">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -11275,16 +11376,16 @@
         <v>13</v>
       </c>
       <c r="B13" s="2">
-        <v>14803</v>
+        <v>14971</v>
       </c>
       <c r="C13" s="2">
-        <v>622.73858642578125</v>
+        <v>629.8060302734375</v>
       </c>
       <c r="D13" s="2">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="E13" s="2">
-        <v>2157</v>
+        <v>2159</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -11292,13 +11393,13 @@
         <v>14</v>
       </c>
       <c r="B14" s="2">
-        <v>1669</v>
+        <v>1673</v>
       </c>
       <c r="C14" s="2">
-        <v>560.9329833984375</v>
+        <v>562.27734375</v>
       </c>
       <c r="D14" s="2">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E14" s="2">
         <v>230</v>
@@ -11309,16 +11410,16 @@
         <v>15</v>
       </c>
       <c r="B15" s="2">
-        <v>2244</v>
+        <v>2262</v>
       </c>
       <c r="C15" s="2">
-        <v>584.81207275390625</v>
+        <v>589.50311279296875</v>
       </c>
       <c r="D15" s="2">
         <v>132</v>
       </c>
       <c r="E15" s="2">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -11326,16 +11427,16 @@
         <v>16</v>
       </c>
       <c r="B16" s="2">
-        <v>641</v>
+        <v>662</v>
       </c>
       <c r="C16" s="2">
-        <v>226.97175598144531</v>
+        <v>234.40763854980469</v>
       </c>
       <c r="D16" s="2">
         <v>26</v>
       </c>
       <c r="E16" s="2">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -11343,10 +11444,10 @@
         <v>17</v>
       </c>
       <c r="B17" s="2">
-        <v>535</v>
+        <v>539</v>
       </c>
       <c r="C17" s="2">
-        <v>196.88226318359375</v>
+        <v>198.35427856445313</v>
       </c>
       <c r="D17" s="2">
         <v>29</v>
@@ -11360,10 +11461,10 @@
         <v>18</v>
       </c>
       <c r="B18" s="2">
-        <v>887</v>
+        <v>905</v>
       </c>
       <c r="C18" s="2">
-        <v>361.52877807617188</v>
+        <v>368.86532592773438</v>
       </c>
       <c r="D18" s="2">
         <v>41</v>
@@ -11377,13 +11478,13 @@
         <v>19</v>
       </c>
       <c r="B19" s="2">
-        <v>1457</v>
+        <v>1527</v>
       </c>
       <c r="C19" s="2">
-        <v>528.1951904296875</v>
+        <v>553.57177734375</v>
       </c>
       <c r="D19" s="2">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E19" s="2">
         <v>148</v>
@@ -11394,16 +11495,16 @@
         <v>29</v>
       </c>
       <c r="B20" s="2">
-        <v>8128</v>
+        <v>8383</v>
       </c>
       <c r="C20" s="2">
-        <v>470.9478759765625</v>
+        <v>485.72293090820313</v>
       </c>
       <c r="D20" s="2">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="E20" s="2">
-        <v>602</v>
+        <v>604</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -11411,10 +11512,10 @@
         <v>21</v>
       </c>
       <c r="B21" s="2">
-        <v>1975</v>
+        <v>1983</v>
       </c>
       <c r="C21" s="2">
-        <v>647.95526123046875</v>
+        <v>650.57989501953125</v>
       </c>
       <c r="D21" s="2">
         <v>73</v>
@@ -11428,13 +11529,13 @@
         <v>22</v>
       </c>
       <c r="B22" s="2">
-        <v>2260</v>
+        <v>2287</v>
       </c>
       <c r="C22" s="2">
-        <v>485.50466918945313</v>
+        <v>491.30496215820313</v>
       </c>
       <c r="D22" s="2">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E22" s="2">
         <v>198</v>
@@ -11450,7 +11551,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -11474,13 +11575,13 @@
         <v>34</v>
       </c>
       <c r="B2" s="2">
-        <v>17996</v>
+        <v>18352</v>
       </c>
       <c r="C2" s="2">
-        <v>1616</v>
+        <v>1627</v>
       </c>
       <c r="D2" s="2">
-        <v>2575</v>
+        <v>2588</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -11488,13 +11589,13 @@
         <v>35</v>
       </c>
       <c r="B3" s="2">
-        <v>27136</v>
+        <v>27571</v>
       </c>
       <c r="C3" s="2">
-        <v>575</v>
+        <v>582</v>
       </c>
       <c r="D3" s="2">
-        <v>2119</v>
+        <v>2129</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -11523,6 +11624,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="13.08984375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -11543,7 +11647,7 @@
         <v>38</v>
       </c>
       <c r="B2" s="2">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C2" s="2">
         <v>5</v>
@@ -11557,7 +11661,7 @@
         <v>39</v>
       </c>
       <c r="B3" s="2">
-        <v>628</v>
+        <v>659</v>
       </c>
       <c r="C3" s="2">
         <v>9</v>
@@ -11571,7 +11675,7 @@
         <v>40</v>
       </c>
       <c r="B4" s="2">
-        <v>4543</v>
+        <v>4631</v>
       </c>
       <c r="C4" s="2">
         <v>81</v>
@@ -11585,7 +11689,7 @@
         <v>41</v>
       </c>
       <c r="B5" s="2">
-        <v>6020</v>
+        <v>6165</v>
       </c>
       <c r="C5" s="2">
         <v>98</v>
@@ -11599,10 +11703,10 @@
         <v>42</v>
       </c>
       <c r="B6" s="2">
-        <v>7061</v>
+        <v>7236</v>
       </c>
       <c r="C6" s="2">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="D6" s="2">
         <v>42</v>
@@ -11613,13 +11717,13 @@
         <v>43</v>
       </c>
       <c r="B7" s="2">
-        <v>8389</v>
+        <v>8541</v>
       </c>
       <c r="C7" s="2">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="D7" s="2">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -11627,13 +11731,13 @@
         <v>44</v>
       </c>
       <c r="B8" s="2">
-        <v>5349</v>
+        <v>5425</v>
       </c>
       <c r="C8" s="2">
-        <v>658</v>
+        <v>667</v>
       </c>
       <c r="D8" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -11641,10 +11745,10 @@
         <v>45</v>
       </c>
       <c r="B9" s="2">
-        <v>4451</v>
+        <v>4508</v>
       </c>
       <c r="C9" s="2">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="D9" s="2">
         <v>1031</v>
@@ -11655,13 +11759,13 @@
         <v>46</v>
       </c>
       <c r="B10" s="2">
-        <v>5463</v>
+        <v>5506</v>
       </c>
       <c r="C10" s="2">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D10" s="2">
-        <v>1930</v>
+        <v>1943</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -11669,13 +11773,13 @@
         <v>47</v>
       </c>
       <c r="B11" s="2">
-        <v>2994</v>
+        <v>3017</v>
       </c>
       <c r="C11" s="2">
         <v>1</v>
       </c>
       <c r="D11" s="2">
-        <v>1193</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -11683,7 +11787,7 @@
         <v>36</v>
       </c>
       <c r="B12" s="2">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" s="2">
         <v>0</v>
@@ -11701,7 +11805,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-09 12:10) (#99)
Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/output/snapshot/9c24c2d6-bc87-568a-aff3-c42f38603962.xlsx
+++ b/output/snapshot/9c24c2d6-bc87-568a-aff3-c42f38603962.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15480" windowHeight="7030" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19350" windowHeight="11470" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Antal per dag region" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Totalt antal per region" sheetId="4" r:id="rId4"/>
     <sheet name="Totalt antal per kön" sheetId="5" r:id="rId5"/>
     <sheet name="Totalt antal per åldersgrupp" sheetId="6" r:id="rId6"/>
-    <sheet name="FOHM  8 Jun 2020" sheetId="7" r:id="rId7"/>
+    <sheet name="FOHM  9 Jun 2020" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -505,15 +505,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W127"/>
+  <dimension ref="A1:W128"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="B33" sqref="B1:B1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="14.1796875" customWidth="1"/>
+    <col min="1" max="1" width="21.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
@@ -8757,7 +8757,7 @@
         <v>43980</v>
       </c>
       <c r="B117" s="2">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="C117" s="2">
         <v>10</v>
@@ -8793,7 +8793,7 @@
         <v>46</v>
       </c>
       <c r="N117" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="O117" s="2">
         <v>4</v>
@@ -9041,7 +9041,7 @@
         <v>43984</v>
       </c>
       <c r="B121" s="2">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="C121" s="2">
         <v>18</v>
@@ -9092,7 +9092,7 @@
         <v>8</v>
       </c>
       <c r="S121" s="2">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="T121" s="2">
         <v>35</v>
@@ -9254,7 +9254,7 @@
         <v>43987</v>
       </c>
       <c r="B124" s="2">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C124" s="2">
         <v>10</v>
@@ -9317,7 +9317,7 @@
         <v>46</v>
       </c>
       <c r="W124" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="125" spans="1:23">
@@ -9325,7 +9325,7 @@
         <v>43988</v>
       </c>
       <c r="B125" s="2">
-        <v>823</v>
+        <v>825</v>
       </c>
       <c r="C125" s="2">
         <v>5</v>
@@ -9334,10 +9334,10 @@
         <v>16</v>
       </c>
       <c r="E125" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F125" s="2">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G125" s="2">
         <v>19</v>
@@ -9361,7 +9361,7 @@
         <v>23</v>
       </c>
       <c r="N125" s="2">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="O125" s="2">
         <v>1</v>
@@ -9388,7 +9388,7 @@
         <v>19</v>
       </c>
       <c r="W125" s="2">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="126" spans="1:23">
@@ -9396,28 +9396,28 @@
         <v>43989</v>
       </c>
       <c r="B126" s="2">
-        <v>344</v>
+        <v>462</v>
       </c>
       <c r="C126" s="2">
         <v>18</v>
       </c>
       <c r="D126" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E126" s="2">
         <v>0</v>
       </c>
       <c r="F126" s="2">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="G126" s="2">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H126" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I126" s="2">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="J126" s="2">
         <v>3</v>
@@ -9432,34 +9432,34 @@
         <v>12</v>
       </c>
       <c r="N126" s="2">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="O126" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P126" s="2">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="Q126" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R126" s="2">
         <v>4</v>
       </c>
       <c r="S126" s="2">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="T126" s="2">
         <v>0</v>
       </c>
       <c r="U126" s="2">
-        <v>170</v>
+        <v>229</v>
       </c>
       <c r="V126" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="W126" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="127" spans="1:23">
@@ -9467,70 +9467,141 @@
         <v>43990</v>
       </c>
       <c r="B127" s="2">
-        <v>68</v>
+        <v>536</v>
       </c>
       <c r="C127" s="2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D127" s="2">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E127" s="2">
         <v>0</v>
       </c>
       <c r="F127" s="2">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="G127" s="2">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="H127" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I127" s="2">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="J127" s="2">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="K127" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L127" s="2">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="M127" s="2">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="N127" s="2">
-        <v>19</v>
+        <v>128</v>
       </c>
       <c r="O127" s="2">
         <v>10</v>
       </c>
       <c r="P127" s="2">
+        <v>12</v>
+      </c>
+      <c r="Q127" s="2">
+        <v>15</v>
+      </c>
+      <c r="R127" s="2">
+        <v>4</v>
+      </c>
+      <c r="S127" s="2">
+        <v>23</v>
+      </c>
+      <c r="T127" s="2">
+        <v>67</v>
+      </c>
+      <c r="U127" s="2">
+        <v>121</v>
+      </c>
+      <c r="V127" s="2">
         <v>7</v>
       </c>
-      <c r="Q127" s="2">
-        <v>0</v>
-      </c>
-      <c r="R127" s="2">
-        <v>0</v>
-      </c>
-      <c r="S127" s="2">
+      <c r="W127" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:23">
+      <c r="A128" s="1">
+        <v>43991</v>
+      </c>
+      <c r="B128" s="2">
+        <v>202</v>
+      </c>
+      <c r="C128" s="2">
+        <v>0</v>
+      </c>
+      <c r="D128" s="2">
+        <v>1</v>
+      </c>
+      <c r="E128" s="2">
+        <v>0</v>
+      </c>
+      <c r="F128" s="2">
+        <v>0</v>
+      </c>
+      <c r="G128" s="2">
+        <v>4</v>
+      </c>
+      <c r="H128" s="2">
         <v>6</v>
       </c>
-      <c r="T127" s="2">
+      <c r="I128" s="2">
+        <v>6</v>
+      </c>
+      <c r="J128" s="2">
+        <v>0</v>
+      </c>
+      <c r="K128" s="2">
+        <v>0</v>
+      </c>
+      <c r="L128" s="2">
+        <v>1</v>
+      </c>
+      <c r="M128" s="2">
+        <v>0</v>
+      </c>
+      <c r="N128" s="2">
+        <v>42</v>
+      </c>
+      <c r="O128" s="2">
+        <v>2</v>
+      </c>
+      <c r="P128" s="2">
+        <v>11</v>
+      </c>
+      <c r="Q128" s="2">
+        <v>5</v>
+      </c>
+      <c r="R128" s="2">
+        <v>0</v>
+      </c>
+      <c r="S128" s="2">
+        <v>1</v>
+      </c>
+      <c r="T128" s="2">
+        <v>24</v>
+      </c>
+      <c r="U128" s="2">
+        <v>78</v>
+      </c>
+      <c r="V128" s="2">
+        <v>0</v>
+      </c>
+      <c r="W128" s="2">
         <v>21</v>
-      </c>
-      <c r="U127" s="2">
-        <v>3</v>
-      </c>
-      <c r="V127" s="2">
-        <v>0</v>
-      </c>
-      <c r="W127" s="2">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -9540,13 +9611,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B91"/>
+  <dimension ref="A1:B93"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="A91" sqref="A91"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="12.90625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -10193,7 +10267,7 @@
         <v>43980</v>
       </c>
       <c r="B81" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -10217,7 +10291,7 @@
         <v>43983</v>
       </c>
       <c r="B84" s="2">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -10233,7 +10307,7 @@
         <v>43985</v>
       </c>
       <c r="B86" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -10249,7 +10323,7 @@
         <v>43987</v>
       </c>
       <c r="B88" s="2">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -10257,7 +10331,7 @@
         <v>43988</v>
       </c>
       <c r="B89" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -10265,15 +10339,31 @@
         <v>43989</v>
       </c>
       <c r="B90" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="91" spans="1:2">
-      <c r="A91" s="1" t="s">
+      <c r="A91" s="1">
+        <v>43990</v>
+      </c>
+      <c r="B91" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" s="1">
+        <v>43991</v>
+      </c>
+      <c r="B92" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B91" s="2">
-        <v>11</v>
+      <c r="B93" s="2">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -10283,13 +10373,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B95"/>
+  <dimension ref="A1:B96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -10392,7 +10485,7 @@
         <v>43907</v>
       </c>
       <c r="B13" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -10472,7 +10565,7 @@
         <v>43917</v>
       </c>
       <c r="B23" s="2">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -10560,7 +10653,7 @@
         <v>43928</v>
       </c>
       <c r="B34" s="2">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -10568,7 +10661,7 @@
         <v>43929</v>
       </c>
       <c r="B35" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -11016,7 +11109,7 @@
         <v>43985</v>
       </c>
       <c r="B91" s="2">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -11024,7 +11117,7 @@
         <v>43986</v>
       </c>
       <c r="B92" s="2">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -11032,7 +11125,7 @@
         <v>43987</v>
       </c>
       <c r="B93" s="2">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -11040,7 +11133,7 @@
         <v>43988</v>
       </c>
       <c r="B94" s="2">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -11048,7 +11141,15 @@
         <v>43989</v>
       </c>
       <c r="B95" s="2">
-        <v>9</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" s="1">
+        <v>43990</v>
+      </c>
+      <c r="B96" s="2">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -11088,16 +11189,16 @@
         <v>2</v>
       </c>
       <c r="B2" s="2">
-        <v>297</v>
+        <v>307</v>
       </c>
       <c r="C2" s="2">
-        <v>186.08323669433594</v>
+        <v>192.34866333007813</v>
       </c>
       <c r="D2" s="2">
         <v>4</v>
       </c>
       <c r="E2" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -11105,10 +11206,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>1315</v>
+        <v>1329</v>
       </c>
       <c r="C3" s="2">
-        <v>456.651123046875</v>
+        <v>461.5128173828125</v>
       </c>
       <c r="D3" s="2">
         <v>61</v>
@@ -11122,10 +11223,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C4" s="2">
-        <v>150.78912353515625</v>
+        <v>152.46456909179688</v>
       </c>
       <c r="D4" s="2">
         <v>5</v>
@@ -11139,16 +11240,16 @@
         <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>1516</v>
+        <v>1542</v>
       </c>
       <c r="C5" s="2">
-        <v>527.5208740234375</v>
+        <v>536.56805419921875</v>
       </c>
       <c r="D5" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E5" s="2">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -11156,13 +11257,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="2">
-        <v>920</v>
+        <v>937</v>
       </c>
       <c r="C6" s="2">
-        <v>275.57452392578125</v>
+        <v>280.66665649414063</v>
       </c>
       <c r="D6" s="2">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E6" s="2">
         <v>57</v>
@@ -11173,10 +11274,10 @@
         <v>28</v>
       </c>
       <c r="B7" s="2">
-        <v>809</v>
+        <v>817</v>
       </c>
       <c r="C7" s="2">
-        <v>618.4542236328125</v>
+        <v>624.57000732421875</v>
       </c>
       <c r="D7" s="2">
         <v>16</v>
@@ -11190,16 +11291,16 @@
         <v>8</v>
       </c>
       <c r="B8" s="2">
-        <v>1751</v>
+        <v>1792</v>
       </c>
       <c r="C8" s="2">
-        <v>481.57449340820313</v>
+        <v>492.85064697265625</v>
       </c>
       <c r="D8" s="2">
         <v>78</v>
       </c>
       <c r="E8" s="2">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -11207,16 +11308,16 @@
         <v>9</v>
       </c>
       <c r="B9" s="2">
-        <v>408</v>
+        <v>421</v>
       </c>
       <c r="C9" s="2">
-        <v>166.22801208496094</v>
+        <v>171.52449035644531</v>
       </c>
       <c r="D9" s="2">
         <v>27</v>
       </c>
       <c r="E9" s="2">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -11224,16 +11325,16 @@
         <v>10</v>
       </c>
       <c r="B10" s="2">
-        <v>930</v>
+        <v>935</v>
       </c>
       <c r="C10" s="2">
-        <v>461.60946655273438</v>
+        <v>464.09124755859375</v>
       </c>
       <c r="D10" s="2">
         <v>17</v>
       </c>
       <c r="E10" s="2">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -11241,16 +11342,16 @@
         <v>11</v>
       </c>
       <c r="B11" s="2">
-        <v>503</v>
+        <v>533</v>
       </c>
       <c r="C11" s="2">
-        <v>201.12518310546875</v>
+        <v>213.12071228027344</v>
       </c>
       <c r="D11" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E11" s="2">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -11258,16 +11359,16 @@
         <v>12</v>
       </c>
       <c r="B12" s="2">
-        <v>1995</v>
+        <v>2028</v>
       </c>
       <c r="C12" s="2">
-        <v>144.793212890625</v>
+        <v>147.18829345703125</v>
       </c>
       <c r="D12" s="2">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="E12" s="2">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -11275,16 +11376,16 @@
         <v>13</v>
       </c>
       <c r="B13" s="2">
-        <v>14803</v>
+        <v>14971</v>
       </c>
       <c r="C13" s="2">
-        <v>622.73858642578125</v>
+        <v>629.8060302734375</v>
       </c>
       <c r="D13" s="2">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="E13" s="2">
-        <v>2157</v>
+        <v>2159</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -11292,13 +11393,13 @@
         <v>14</v>
       </c>
       <c r="B14" s="2">
-        <v>1669</v>
+        <v>1673</v>
       </c>
       <c r="C14" s="2">
-        <v>560.9329833984375</v>
+        <v>562.27734375</v>
       </c>
       <c r="D14" s="2">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E14" s="2">
         <v>230</v>
@@ -11309,16 +11410,16 @@
         <v>15</v>
       </c>
       <c r="B15" s="2">
-        <v>2244</v>
+        <v>2262</v>
       </c>
       <c r="C15" s="2">
-        <v>584.81207275390625</v>
+        <v>589.50311279296875</v>
       </c>
       <c r="D15" s="2">
         <v>132</v>
       </c>
       <c r="E15" s="2">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -11326,16 +11427,16 @@
         <v>16</v>
       </c>
       <c r="B16" s="2">
-        <v>641</v>
+        <v>662</v>
       </c>
       <c r="C16" s="2">
-        <v>226.97175598144531</v>
+        <v>234.40763854980469</v>
       </c>
       <c r="D16" s="2">
         <v>26</v>
       </c>
       <c r="E16" s="2">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -11343,10 +11444,10 @@
         <v>17</v>
       </c>
       <c r="B17" s="2">
-        <v>535</v>
+        <v>539</v>
       </c>
       <c r="C17" s="2">
-        <v>196.88226318359375</v>
+        <v>198.35427856445313</v>
       </c>
       <c r="D17" s="2">
         <v>29</v>
@@ -11360,10 +11461,10 @@
         <v>18</v>
       </c>
       <c r="B18" s="2">
-        <v>887</v>
+        <v>905</v>
       </c>
       <c r="C18" s="2">
-        <v>361.52877807617188</v>
+        <v>368.86532592773438</v>
       </c>
       <c r="D18" s="2">
         <v>41</v>
@@ -11377,13 +11478,13 @@
         <v>19</v>
       </c>
       <c r="B19" s="2">
-        <v>1457</v>
+        <v>1527</v>
       </c>
       <c r="C19" s="2">
-        <v>528.1951904296875</v>
+        <v>553.57177734375</v>
       </c>
       <c r="D19" s="2">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E19" s="2">
         <v>148</v>
@@ -11394,16 +11495,16 @@
         <v>29</v>
       </c>
       <c r="B20" s="2">
-        <v>8128</v>
+        <v>8383</v>
       </c>
       <c r="C20" s="2">
-        <v>470.9478759765625</v>
+        <v>485.72293090820313</v>
       </c>
       <c r="D20" s="2">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="E20" s="2">
-        <v>602</v>
+        <v>604</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -11411,10 +11512,10 @@
         <v>21</v>
       </c>
       <c r="B21" s="2">
-        <v>1975</v>
+        <v>1983</v>
       </c>
       <c r="C21" s="2">
-        <v>647.95526123046875</v>
+        <v>650.57989501953125</v>
       </c>
       <c r="D21" s="2">
         <v>73</v>
@@ -11428,13 +11529,13 @@
         <v>22</v>
       </c>
       <c r="B22" s="2">
-        <v>2260</v>
+        <v>2287</v>
       </c>
       <c r="C22" s="2">
-        <v>485.50466918945313</v>
+        <v>491.30496215820313</v>
       </c>
       <c r="D22" s="2">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E22" s="2">
         <v>198</v>
@@ -11450,7 +11551,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -11474,13 +11575,13 @@
         <v>34</v>
       </c>
       <c r="B2" s="2">
-        <v>17996</v>
+        <v>18352</v>
       </c>
       <c r="C2" s="2">
-        <v>1616</v>
+        <v>1627</v>
       </c>
       <c r="D2" s="2">
-        <v>2575</v>
+        <v>2588</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -11488,13 +11589,13 @@
         <v>35</v>
       </c>
       <c r="B3" s="2">
-        <v>27136</v>
+        <v>27571</v>
       </c>
       <c r="C3" s="2">
-        <v>575</v>
+        <v>582</v>
       </c>
       <c r="D3" s="2">
-        <v>2119</v>
+        <v>2129</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -11523,6 +11624,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="13.08984375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -11543,7 +11647,7 @@
         <v>38</v>
       </c>
       <c r="B2" s="2">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C2" s="2">
         <v>5</v>
@@ -11557,7 +11661,7 @@
         <v>39</v>
       </c>
       <c r="B3" s="2">
-        <v>628</v>
+        <v>659</v>
       </c>
       <c r="C3" s="2">
         <v>9</v>
@@ -11571,7 +11675,7 @@
         <v>40</v>
       </c>
       <c r="B4" s="2">
-        <v>4543</v>
+        <v>4631</v>
       </c>
       <c r="C4" s="2">
         <v>81</v>
@@ -11585,7 +11689,7 @@
         <v>41</v>
       </c>
       <c r="B5" s="2">
-        <v>6020</v>
+        <v>6165</v>
       </c>
       <c r="C5" s="2">
         <v>98</v>
@@ -11599,10 +11703,10 @@
         <v>42</v>
       </c>
       <c r="B6" s="2">
-        <v>7061</v>
+        <v>7236</v>
       </c>
       <c r="C6" s="2">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="D6" s="2">
         <v>42</v>
@@ -11613,13 +11717,13 @@
         <v>43</v>
       </c>
       <c r="B7" s="2">
-        <v>8389</v>
+        <v>8541</v>
       </c>
       <c r="C7" s="2">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="D7" s="2">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -11627,13 +11731,13 @@
         <v>44</v>
       </c>
       <c r="B8" s="2">
-        <v>5349</v>
+        <v>5425</v>
       </c>
       <c r="C8" s="2">
-        <v>658</v>
+        <v>667</v>
       </c>
       <c r="D8" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -11641,10 +11745,10 @@
         <v>45</v>
       </c>
       <c r="B9" s="2">
-        <v>4451</v>
+        <v>4508</v>
       </c>
       <c r="C9" s="2">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="D9" s="2">
         <v>1031</v>
@@ -11655,13 +11759,13 @@
         <v>46</v>
       </c>
       <c r="B10" s="2">
-        <v>5463</v>
+        <v>5506</v>
       </c>
       <c r="C10" s="2">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D10" s="2">
-        <v>1930</v>
+        <v>1943</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -11669,13 +11773,13 @@
         <v>47</v>
       </c>
       <c r="B11" s="2">
-        <v>2994</v>
+        <v>3017</v>
       </c>
       <c r="C11" s="2">
         <v>1</v>
       </c>
       <c r="D11" s="2">
-        <v>1193</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -11683,7 +11787,7 @@
         <v>36</v>
       </c>
       <c r="B12" s="2">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" s="2">
         <v>0</v>
@@ -11701,7 +11805,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-10 12:09)
</commit_message>
<xml_diff>
--- a/output/snapshot/9c24c2d6-bc87-568a-aff3-c42f38603962.xlsx
+++ b/output/snapshot/9c24c2d6-bc87-568a-aff3-c42f38603962.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19350" windowHeight="11470" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Antal per dag region" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,9 @@
     <sheet name="Totalt antal per region" sheetId="4" r:id="rId4"/>
     <sheet name="Totalt antal per kön" sheetId="5" r:id="rId5"/>
     <sheet name="Totalt antal per åldersgrupp" sheetId="6" r:id="rId6"/>
-    <sheet name="FOHM  9 Jun 2020" sheetId="7" r:id="rId7"/>
+    <sheet name="FOHM 10 Jun 2020" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -221,10 +221,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,15 +506,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W128"/>
+  <dimension ref="A1:W130"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:N1048576"/>
+      <selection activeCell="B130" sqref="B130"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.26953125" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
@@ -8056,7 +8057,7 @@
         <v>2</v>
       </c>
       <c r="E107" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F107" s="2">
         <v>34</v>
@@ -8083,7 +8084,7 @@
         <v>63</v>
       </c>
       <c r="N107" s="2">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="O107" s="2">
         <v>18</v>
@@ -9467,7 +9468,7 @@
         <v>43990</v>
       </c>
       <c r="B127" s="2">
-        <v>536</v>
+        <v>542</v>
       </c>
       <c r="C127" s="2">
         <v>10</v>
@@ -9497,7 +9498,7 @@
         <v>5</v>
       </c>
       <c r="L127" s="2">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="M127" s="2">
         <v>33</v>
@@ -9509,7 +9510,7 @@
         <v>10</v>
       </c>
       <c r="P127" s="2">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="Q127" s="2">
         <v>15</v>
@@ -9524,13 +9525,13 @@
         <v>67</v>
       </c>
       <c r="U127" s="2">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="V127" s="2">
         <v>7</v>
       </c>
       <c r="W127" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="128" spans="1:23">
@@ -9538,71 +9539,145 @@
         <v>43991</v>
       </c>
       <c r="B128" s="2">
-        <v>202</v>
+        <v>888</v>
       </c>
       <c r="C128" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D128" s="2">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E128" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F128" s="2">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G128" s="2">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="H128" s="2">
+        <v>17</v>
+      </c>
+      <c r="I128" s="2">
+        <v>62</v>
+      </c>
+      <c r="J128" s="2">
+        <v>12</v>
+      </c>
+      <c r="K128" s="2">
+        <v>15</v>
+      </c>
+      <c r="L128" s="2">
+        <v>3</v>
+      </c>
+      <c r="M128" s="2">
+        <v>44</v>
+      </c>
+      <c r="N128" s="2">
+        <v>217</v>
+      </c>
+      <c r="O128" s="2">
+        <v>3</v>
+      </c>
+      <c r="P128" s="2">
+        <v>48</v>
+      </c>
+      <c r="Q128" s="2">
+        <v>21</v>
+      </c>
+      <c r="R128" s="2">
+        <v>9</v>
+      </c>
+      <c r="S128" s="2">
+        <v>19</v>
+      </c>
+      <c r="T128" s="2">
+        <v>33</v>
+      </c>
+      <c r="U128" s="2">
+        <v>244</v>
+      </c>
+      <c r="V128" s="2">
+        <v>26</v>
+      </c>
+      <c r="W128" s="2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="129" spans="1:23">
+      <c r="A129" s="1">
+        <v>43992</v>
+      </c>
+      <c r="B129" s="2">
+        <v>198</v>
+      </c>
+      <c r="C129" s="2">
+        <v>0</v>
+      </c>
+      <c r="D129" s="2">
+        <v>0</v>
+      </c>
+      <c r="E129" s="2">
+        <v>0</v>
+      </c>
+      <c r="F129" s="2">
+        <v>33</v>
+      </c>
+      <c r="G129" s="2">
+        <v>1</v>
+      </c>
+      <c r="H129" s="2">
+        <v>11</v>
+      </c>
+      <c r="I129" s="2">
+        <v>9</v>
+      </c>
+      <c r="J129" s="2">
+        <v>7</v>
+      </c>
+      <c r="K129" s="2">
+        <v>0</v>
+      </c>
+      <c r="L129" s="2">
+        <v>1</v>
+      </c>
+      <c r="M129" s="2">
+        <v>16</v>
+      </c>
+      <c r="N129" s="2">
+        <v>28</v>
+      </c>
+      <c r="O129" s="2">
+        <v>1</v>
+      </c>
+      <c r="P129" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q129" s="2">
+        <v>0</v>
+      </c>
+      <c r="R129" s="2">
+        <v>0</v>
+      </c>
+      <c r="S129" s="2">
         <v>6</v>
       </c>
-      <c r="I128" s="2">
-        <v>6</v>
-      </c>
-      <c r="J128" s="2">
-        <v>0</v>
-      </c>
-      <c r="K128" s="2">
-        <v>0</v>
-      </c>
-      <c r="L128" s="2">
-        <v>1</v>
-      </c>
-      <c r="M128" s="2">
-        <v>0</v>
-      </c>
-      <c r="N128" s="2">
-        <v>42</v>
-      </c>
-      <c r="O128" s="2">
-        <v>2</v>
-      </c>
-      <c r="P128" s="2">
+      <c r="T129" s="2">
         <v>11</v>
       </c>
-      <c r="Q128" s="2">
-        <v>5</v>
-      </c>
-      <c r="R128" s="2">
-        <v>0</v>
-      </c>
-      <c r="S128" s="2">
-        <v>1</v>
-      </c>
-      <c r="T128" s="2">
-        <v>24</v>
-      </c>
-      <c r="U128" s="2">
-        <v>78</v>
-      </c>
-      <c r="V128" s="2">
-        <v>0</v>
-      </c>
-      <c r="W128" s="2">
-        <v>21</v>
-      </c>
+      <c r="U129" s="2">
+        <v>58</v>
+      </c>
+      <c r="V129" s="2">
+        <v>7</v>
+      </c>
+      <c r="W129" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="130" spans="1:23">
+      <c r="B130" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9611,16 +9686,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B93"/>
+  <dimension ref="A1:B95"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="J96" sqref="J96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="12.90625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -10099,7 +10171,7 @@
         <v>43959</v>
       </c>
       <c r="B60" s="2">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -10107,7 +10179,7 @@
         <v>43960</v>
       </c>
       <c r="B61" s="2">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -10155,7 +10227,7 @@
         <v>43966</v>
       </c>
       <c r="B67" s="2">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -10163,7 +10235,7 @@
         <v>43967</v>
       </c>
       <c r="B68" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -10179,7 +10251,7 @@
         <v>43969</v>
       </c>
       <c r="B70" s="2">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -10227,7 +10299,7 @@
         <v>43975</v>
       </c>
       <c r="B76" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -10235,7 +10307,7 @@
         <v>43976</v>
       </c>
       <c r="B77" s="2">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -10243,7 +10315,7 @@
         <v>43977</v>
       </c>
       <c r="B78" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -10251,7 +10323,7 @@
         <v>43978</v>
       </c>
       <c r="B79" s="2">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -10259,7 +10331,7 @@
         <v>43979</v>
       </c>
       <c r="B80" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -10267,7 +10339,7 @@
         <v>43980</v>
       </c>
       <c r="B81" s="2">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -10275,7 +10347,7 @@
         <v>43981</v>
       </c>
       <c r="B82" s="2">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -10283,7 +10355,7 @@
         <v>43982</v>
       </c>
       <c r="B83" s="2">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -10291,7 +10363,7 @@
         <v>43983</v>
       </c>
       <c r="B84" s="2">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -10299,7 +10371,7 @@
         <v>43984</v>
       </c>
       <c r="B85" s="2">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -10307,7 +10379,7 @@
         <v>43985</v>
       </c>
       <c r="B86" s="2">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -10315,7 +10387,7 @@
         <v>43986</v>
       </c>
       <c r="B87" s="2">
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -10323,7 +10395,7 @@
         <v>43987</v>
       </c>
       <c r="B88" s="2">
-        <v>9</v>
+        <v>20</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -10331,7 +10403,7 @@
         <v>43988</v>
       </c>
       <c r="B89" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -10339,7 +10411,7 @@
         <v>43989</v>
       </c>
       <c r="B90" s="2">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -10347,7 +10419,7 @@
         <v>43990</v>
       </c>
       <c r="B91" s="2">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -10355,16 +10427,27 @@
         <v>43991</v>
       </c>
       <c r="B92" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="93" spans="1:2">
-      <c r="A93" s="1" t="s">
+      <c r="A93" s="1">
+        <v>43992</v>
+      </c>
+      <c r="B93" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B93" s="2">
-        <v>12</v>
-      </c>
+      <c r="B94" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="B95" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10373,16 +10456,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B96"/>
+  <dimension ref="A1:B99"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="I102" sqref="I102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="13" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -11109,7 +11189,7 @@
         <v>43985</v>
       </c>
       <c r="B91" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -11125,7 +11205,7 @@
         <v>43987</v>
       </c>
       <c r="B93" s="2">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -11133,7 +11213,7 @@
         <v>43988</v>
       </c>
       <c r="B94" s="2">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -11141,7 +11221,7 @@
         <v>43989</v>
       </c>
       <c r="B95" s="2">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -11149,8 +11229,27 @@
         <v>43990</v>
       </c>
       <c r="B96" s="2">
-        <v>6</v>
-      </c>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" s="1">
+        <v>43991</v>
+      </c>
+      <c r="B97" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" s="1">
+        <v>43992</v>
+      </c>
+      <c r="B98" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="B99" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11159,13 +11258,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -11189,10 +11288,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="2">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="C2" s="2">
-        <v>192.34866333007813</v>
+        <v>194.85482788085938</v>
       </c>
       <c r="D2" s="2">
         <v>4</v>
@@ -11206,16 +11305,16 @@
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>1329</v>
+        <v>1345</v>
       </c>
       <c r="C3" s="2">
-        <v>461.5128173828125</v>
+        <v>467.06903076171875</v>
       </c>
       <c r="D3" s="2">
         <v>61</v>
       </c>
       <c r="E3" s="2">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -11223,10 +11322,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="2">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="C4" s="2">
-        <v>152.46456909179688</v>
+        <v>162.51716613769531</v>
       </c>
       <c r="D4" s="2">
         <v>5</v>
@@ -11240,16 +11339,16 @@
         <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>1542</v>
+        <v>1587</v>
       </c>
       <c r="C5" s="2">
-        <v>536.56805419921875</v>
+        <v>552.22662353515625</v>
       </c>
       <c r="D5" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E5" s="2">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -11257,16 +11356,16 @@
         <v>6</v>
       </c>
       <c r="B6" s="2">
-        <v>937</v>
+        <v>963</v>
       </c>
       <c r="C6" s="2">
-        <v>280.66665649414063</v>
+        <v>288.45462036132813</v>
       </c>
       <c r="D6" s="2">
         <v>33</v>
       </c>
       <c r="E6" s="2">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -11274,10 +11373,10 @@
         <v>28</v>
       </c>
       <c r="B7" s="2">
-        <v>817</v>
+        <v>839</v>
       </c>
       <c r="C7" s="2">
-        <v>624.57000732421875</v>
+        <v>641.38824462890625</v>
       </c>
       <c r="D7" s="2">
         <v>16</v>
@@ -11291,16 +11390,16 @@
         <v>8</v>
       </c>
       <c r="B8" s="2">
-        <v>1792</v>
+        <v>1857</v>
       </c>
       <c r="C8" s="2">
-        <v>492.85064697265625</v>
+        <v>510.72747802734375</v>
       </c>
       <c r="D8" s="2">
         <v>78</v>
       </c>
       <c r="E8" s="2">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -11308,10 +11407,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="2">
-        <v>421</v>
+        <v>440</v>
       </c>
       <c r="C9" s="2">
-        <v>171.52449035644531</v>
+        <v>179.2655029296875</v>
       </c>
       <c r="D9" s="2">
         <v>27</v>
@@ -11325,16 +11424,16 @@
         <v>10</v>
       </c>
       <c r="B10" s="2">
-        <v>935</v>
+        <v>950</v>
       </c>
       <c r="C10" s="2">
-        <v>464.09124755859375</v>
+        <v>471.53656005859375</v>
       </c>
       <c r="D10" s="2">
         <v>17</v>
       </c>
       <c r="E10" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -11342,16 +11441,16 @@
         <v>11</v>
       </c>
       <c r="B11" s="2">
-        <v>533</v>
+        <v>537</v>
       </c>
       <c r="C11" s="2">
-        <v>213.12071228027344</v>
+        <v>214.72012329101563</v>
       </c>
       <c r="D11" s="2">
         <v>40</v>
       </c>
       <c r="E11" s="2">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -11359,16 +11458,16 @@
         <v>12</v>
       </c>
       <c r="B12" s="2">
-        <v>2028</v>
+        <v>2088</v>
       </c>
       <c r="C12" s="2">
-        <v>147.18829345703125</v>
+        <v>151.54296875</v>
       </c>
       <c r="D12" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E12" s="2">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -11376,16 +11475,16 @@
         <v>13</v>
       </c>
       <c r="B13" s="2">
-        <v>14971</v>
+        <v>15173</v>
       </c>
       <c r="C13" s="2">
-        <v>629.8060302734375</v>
+        <v>638.30389404296875</v>
       </c>
       <c r="D13" s="2">
-        <v>828</v>
+        <v>835</v>
       </c>
       <c r="E13" s="2">
-        <v>2159</v>
+        <v>2178</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -11393,16 +11492,16 @@
         <v>14</v>
       </c>
       <c r="B14" s="2">
-        <v>1673</v>
+        <v>1675</v>
       </c>
       <c r="C14" s="2">
-        <v>562.27734375</v>
+        <v>562.94952392578125</v>
       </c>
       <c r="D14" s="2">
         <v>128</v>
       </c>
       <c r="E14" s="2">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -11410,16 +11509,16 @@
         <v>15</v>
       </c>
       <c r="B15" s="2">
-        <v>2262</v>
+        <v>2302</v>
       </c>
       <c r="C15" s="2">
-        <v>589.50311279296875</v>
+        <v>599.92755126953125</v>
       </c>
       <c r="D15" s="2">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="E15" s="2">
-        <v>185</v>
+        <v>191</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -11427,10 +11526,10 @@
         <v>16</v>
       </c>
       <c r="B16" s="2">
-        <v>662</v>
+        <v>678</v>
       </c>
       <c r="C16" s="2">
-        <v>234.40763854980469</v>
+        <v>240.07308959960938</v>
       </c>
       <c r="D16" s="2">
         <v>26</v>
@@ -11444,13 +11543,13 @@
         <v>17</v>
       </c>
       <c r="B17" s="2">
-        <v>539</v>
+        <v>548</v>
       </c>
       <c r="C17" s="2">
-        <v>198.35427856445313</v>
+        <v>201.66632080078125</v>
       </c>
       <c r="D17" s="2">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E17" s="2">
         <v>29</v>
@@ -11461,16 +11560,16 @@
         <v>18</v>
       </c>
       <c r="B18" s="2">
-        <v>905</v>
+        <v>929</v>
       </c>
       <c r="C18" s="2">
-        <v>368.86532592773438</v>
+        <v>378.64739990234375</v>
       </c>
       <c r="D18" s="2">
         <v>41</v>
       </c>
       <c r="E18" s="2">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -11478,10 +11577,10 @@
         <v>19</v>
       </c>
       <c r="B19" s="2">
-        <v>1527</v>
+        <v>1547</v>
       </c>
       <c r="C19" s="2">
-        <v>553.57177734375</v>
+        <v>560.82220458984375</v>
       </c>
       <c r="D19" s="2">
         <v>49</v>
@@ -11495,16 +11594,16 @@
         <v>29</v>
       </c>
       <c r="B20" s="2">
-        <v>8383</v>
+        <v>8608</v>
       </c>
       <c r="C20" s="2">
-        <v>485.72293090820313</v>
+        <v>498.759765625</v>
       </c>
       <c r="D20" s="2">
-        <v>360</v>
+        <v>367</v>
       </c>
       <c r="E20" s="2">
-        <v>604</v>
+        <v>631</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -11512,16 +11611,16 @@
         <v>21</v>
       </c>
       <c r="B21" s="2">
-        <v>1983</v>
+        <v>2016</v>
       </c>
       <c r="C21" s="2">
-        <v>650.57989501953125</v>
+        <v>661.406494140625</v>
       </c>
       <c r="D21" s="2">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E21" s="2">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -11529,17 +11628,23 @@
         <v>22</v>
       </c>
       <c r="B22" s="2">
-        <v>2287</v>
+        <v>2324</v>
       </c>
       <c r="C22" s="2">
-        <v>491.30496215820313</v>
+        <v>499.25347900390625</v>
       </c>
       <c r="D22" s="2">
         <v>102</v>
       </c>
       <c r="E22" s="2">
-        <v>198</v>
-      </c>
+        <v>201</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11548,15 +11653,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -11570,35 +11675,35 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>34</v>
       </c>
       <c r="B2" s="2">
-        <v>18352</v>
+        <v>18717</v>
       </c>
       <c r="C2" s="2">
-        <v>1627</v>
+        <v>1646</v>
       </c>
       <c r="D2" s="2">
-        <v>2588</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>2631</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>35</v>
       </c>
       <c r="B3" s="2">
-        <v>27571</v>
+        <v>28096</v>
       </c>
       <c r="C3" s="2">
-        <v>582</v>
+        <v>586</v>
       </c>
       <c r="D3" s="2">
-        <v>2129</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>2164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -11611,6 +11716,12 @@
       <c r="D4" s="2">
         <v>0</v>
       </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11623,10 +11734,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="13.08984375" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -11647,7 +11755,7 @@
         <v>38</v>
       </c>
       <c r="B2" s="2">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="C2" s="2">
         <v>5</v>
@@ -11661,7 +11769,7 @@
         <v>39</v>
       </c>
       <c r="B3" s="2">
-        <v>659</v>
+        <v>696</v>
       </c>
       <c r="C3" s="2">
         <v>9</v>
@@ -11675,7 +11783,7 @@
         <v>40</v>
       </c>
       <c r="B4" s="2">
-        <v>4631</v>
+        <v>4756</v>
       </c>
       <c r="C4" s="2">
         <v>81</v>
@@ -11689,10 +11797,10 @@
         <v>41</v>
       </c>
       <c r="B5" s="2">
-        <v>6165</v>
+        <v>6324</v>
       </c>
       <c r="C5" s="2">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D5" s="2">
         <v>12</v>
@@ -11703,10 +11811,10 @@
         <v>42</v>
       </c>
       <c r="B6" s="2">
-        <v>7236</v>
+        <v>7393</v>
       </c>
       <c r="C6" s="2">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="D6" s="2">
         <v>42</v>
@@ -11717,13 +11825,13 @@
         <v>43</v>
       </c>
       <c r="B7" s="2">
-        <v>8541</v>
+        <v>8706</v>
       </c>
       <c r="C7" s="2">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="D7" s="2">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -11731,13 +11839,13 @@
         <v>44</v>
       </c>
       <c r="B8" s="2">
-        <v>5425</v>
+        <v>5511</v>
       </c>
       <c r="C8" s="2">
-        <v>667</v>
+        <v>673</v>
       </c>
       <c r="D8" s="2">
-        <v>340</v>
+        <v>346</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -11745,13 +11853,13 @@
         <v>45</v>
       </c>
       <c r="B9" s="2">
-        <v>4508</v>
+        <v>4559</v>
       </c>
       <c r="C9" s="2">
-        <v>430</v>
+        <v>436</v>
       </c>
       <c r="D9" s="2">
-        <v>1031</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -11759,13 +11867,13 @@
         <v>46</v>
       </c>
       <c r="B10" s="2">
-        <v>5506</v>
+        <v>5575</v>
       </c>
       <c r="C10" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D10" s="2">
-        <v>1943</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -11773,13 +11881,13 @@
         <v>47</v>
       </c>
       <c r="B11" s="2">
-        <v>3017</v>
+        <v>3051</v>
       </c>
       <c r="C11" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11" s="2">
-        <v>1201</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -11805,9 +11913,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-10 12:09) (#104)
Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/output/snapshot/9c24c2d6-bc87-568a-aff3-c42f38603962.xlsx
+++ b/output/snapshot/9c24c2d6-bc87-568a-aff3-c42f38603962.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19350" windowHeight="11470" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Antal per dag region" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,9 @@
     <sheet name="Totalt antal per region" sheetId="4" r:id="rId4"/>
     <sheet name="Totalt antal per kön" sheetId="5" r:id="rId5"/>
     <sheet name="Totalt antal per åldersgrupp" sheetId="6" r:id="rId6"/>
-    <sheet name="FOHM  9 Jun 2020" sheetId="7" r:id="rId7"/>
+    <sheet name="FOHM 10 Jun 2020" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -221,10 +221,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,15 +506,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W128"/>
+  <dimension ref="A1:W130"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:N1048576"/>
+      <selection activeCell="B130" sqref="B130"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.26953125" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
@@ -8056,7 +8057,7 @@
         <v>2</v>
       </c>
       <c r="E107" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F107" s="2">
         <v>34</v>
@@ -8083,7 +8084,7 @@
         <v>63</v>
       </c>
       <c r="N107" s="2">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="O107" s="2">
         <v>18</v>
@@ -9467,7 +9468,7 @@
         <v>43990</v>
       </c>
       <c r="B127" s="2">
-        <v>536</v>
+        <v>542</v>
       </c>
       <c r="C127" s="2">
         <v>10</v>
@@ -9497,7 +9498,7 @@
         <v>5</v>
       </c>
       <c r="L127" s="2">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="M127" s="2">
         <v>33</v>
@@ -9509,7 +9510,7 @@
         <v>10</v>
       </c>
       <c r="P127" s="2">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="Q127" s="2">
         <v>15</v>
@@ -9524,13 +9525,13 @@
         <v>67</v>
       </c>
       <c r="U127" s="2">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="V127" s="2">
         <v>7</v>
       </c>
       <c r="W127" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="128" spans="1:23">
@@ -9538,71 +9539,145 @@
         <v>43991</v>
       </c>
       <c r="B128" s="2">
-        <v>202</v>
+        <v>888</v>
       </c>
       <c r="C128" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D128" s="2">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E128" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F128" s="2">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G128" s="2">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="H128" s="2">
+        <v>17</v>
+      </c>
+      <c r="I128" s="2">
+        <v>62</v>
+      </c>
+      <c r="J128" s="2">
+        <v>12</v>
+      </c>
+      <c r="K128" s="2">
+        <v>15</v>
+      </c>
+      <c r="L128" s="2">
+        <v>3</v>
+      </c>
+      <c r="M128" s="2">
+        <v>44</v>
+      </c>
+      <c r="N128" s="2">
+        <v>217</v>
+      </c>
+      <c r="O128" s="2">
+        <v>3</v>
+      </c>
+      <c r="P128" s="2">
+        <v>48</v>
+      </c>
+      <c r="Q128" s="2">
+        <v>21</v>
+      </c>
+      <c r="R128" s="2">
+        <v>9</v>
+      </c>
+      <c r="S128" s="2">
+        <v>19</v>
+      </c>
+      <c r="T128" s="2">
+        <v>33</v>
+      </c>
+      <c r="U128" s="2">
+        <v>244</v>
+      </c>
+      <c r="V128" s="2">
+        <v>26</v>
+      </c>
+      <c r="W128" s="2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="129" spans="1:23">
+      <c r="A129" s="1">
+        <v>43992</v>
+      </c>
+      <c r="B129" s="2">
+        <v>198</v>
+      </c>
+      <c r="C129" s="2">
+        <v>0</v>
+      </c>
+      <c r="D129" s="2">
+        <v>0</v>
+      </c>
+      <c r="E129" s="2">
+        <v>0</v>
+      </c>
+      <c r="F129" s="2">
+        <v>33</v>
+      </c>
+      <c r="G129" s="2">
+        <v>1</v>
+      </c>
+      <c r="H129" s="2">
+        <v>11</v>
+      </c>
+      <c r="I129" s="2">
+        <v>9</v>
+      </c>
+      <c r="J129" s="2">
+        <v>7</v>
+      </c>
+      <c r="K129" s="2">
+        <v>0</v>
+      </c>
+      <c r="L129" s="2">
+        <v>1</v>
+      </c>
+      <c r="M129" s="2">
+        <v>16</v>
+      </c>
+      <c r="N129" s="2">
+        <v>28</v>
+      </c>
+      <c r="O129" s="2">
+        <v>1</v>
+      </c>
+      <c r="P129" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q129" s="2">
+        <v>0</v>
+      </c>
+      <c r="R129" s="2">
+        <v>0</v>
+      </c>
+      <c r="S129" s="2">
         <v>6</v>
       </c>
-      <c r="I128" s="2">
-        <v>6</v>
-      </c>
-      <c r="J128" s="2">
-        <v>0</v>
-      </c>
-      <c r="K128" s="2">
-        <v>0</v>
-      </c>
-      <c r="L128" s="2">
-        <v>1</v>
-      </c>
-      <c r="M128" s="2">
-        <v>0</v>
-      </c>
-      <c r="N128" s="2">
-        <v>42</v>
-      </c>
-      <c r="O128" s="2">
-        <v>2</v>
-      </c>
-      <c r="P128" s="2">
+      <c r="T129" s="2">
         <v>11</v>
       </c>
-      <c r="Q128" s="2">
-        <v>5</v>
-      </c>
-      <c r="R128" s="2">
-        <v>0</v>
-      </c>
-      <c r="S128" s="2">
-        <v>1</v>
-      </c>
-      <c r="T128" s="2">
-        <v>24</v>
-      </c>
-      <c r="U128" s="2">
-        <v>78</v>
-      </c>
-      <c r="V128" s="2">
-        <v>0</v>
-      </c>
-      <c r="W128" s="2">
-        <v>21</v>
-      </c>
+      <c r="U129" s="2">
+        <v>58</v>
+      </c>
+      <c r="V129" s="2">
+        <v>7</v>
+      </c>
+      <c r="W129" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="130" spans="1:23">
+      <c r="B130" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9611,16 +9686,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B93"/>
+  <dimension ref="A1:B95"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="J96" sqref="J96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="12.90625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -10099,7 +10171,7 @@
         <v>43959</v>
       </c>
       <c r="B60" s="2">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -10107,7 +10179,7 @@
         <v>43960</v>
       </c>
       <c r="B61" s="2">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -10155,7 +10227,7 @@
         <v>43966</v>
       </c>
       <c r="B67" s="2">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -10163,7 +10235,7 @@
         <v>43967</v>
       </c>
       <c r="B68" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -10179,7 +10251,7 @@
         <v>43969</v>
       </c>
       <c r="B70" s="2">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -10227,7 +10299,7 @@
         <v>43975</v>
       </c>
       <c r="B76" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -10235,7 +10307,7 @@
         <v>43976</v>
       </c>
       <c r="B77" s="2">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -10243,7 +10315,7 @@
         <v>43977</v>
       </c>
       <c r="B78" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -10251,7 +10323,7 @@
         <v>43978</v>
       </c>
       <c r="B79" s="2">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -10259,7 +10331,7 @@
         <v>43979</v>
       </c>
       <c r="B80" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -10267,7 +10339,7 @@
         <v>43980</v>
       </c>
       <c r="B81" s="2">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -10275,7 +10347,7 @@
         <v>43981</v>
       </c>
       <c r="B82" s="2">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -10283,7 +10355,7 @@
         <v>43982</v>
       </c>
       <c r="B83" s="2">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -10291,7 +10363,7 @@
         <v>43983</v>
       </c>
       <c r="B84" s="2">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -10299,7 +10371,7 @@
         <v>43984</v>
       </c>
       <c r="B85" s="2">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -10307,7 +10379,7 @@
         <v>43985</v>
       </c>
       <c r="B86" s="2">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -10315,7 +10387,7 @@
         <v>43986</v>
       </c>
       <c r="B87" s="2">
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -10323,7 +10395,7 @@
         <v>43987</v>
       </c>
       <c r="B88" s="2">
-        <v>9</v>
+        <v>20</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -10331,7 +10403,7 @@
         <v>43988</v>
       </c>
       <c r="B89" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -10339,7 +10411,7 @@
         <v>43989</v>
       </c>
       <c r="B90" s="2">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -10347,7 +10419,7 @@
         <v>43990</v>
       </c>
       <c r="B91" s="2">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -10355,16 +10427,27 @@
         <v>43991</v>
       </c>
       <c r="B92" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="93" spans="1:2">
-      <c r="A93" s="1" t="s">
+      <c r="A93" s="1">
+        <v>43992</v>
+      </c>
+      <c r="B93" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B93" s="2">
-        <v>12</v>
-      </c>
+      <c r="B94" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="B95" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10373,16 +10456,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B96"/>
+  <dimension ref="A1:B99"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="I102" sqref="I102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="13" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -11109,7 +11189,7 @@
         <v>43985</v>
       </c>
       <c r="B91" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -11125,7 +11205,7 @@
         <v>43987</v>
       </c>
       <c r="B93" s="2">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -11133,7 +11213,7 @@
         <v>43988</v>
       </c>
       <c r="B94" s="2">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -11141,7 +11221,7 @@
         <v>43989</v>
       </c>
       <c r="B95" s="2">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -11149,8 +11229,27 @@
         <v>43990</v>
       </c>
       <c r="B96" s="2">
-        <v>6</v>
-      </c>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" s="1">
+        <v>43991</v>
+      </c>
+      <c r="B97" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" s="1">
+        <v>43992</v>
+      </c>
+      <c r="B98" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="B99" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11159,13 +11258,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -11189,10 +11288,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="2">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="C2" s="2">
-        <v>192.34866333007813</v>
+        <v>194.85482788085938</v>
       </c>
       <c r="D2" s="2">
         <v>4</v>
@@ -11206,16 +11305,16 @@
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>1329</v>
+        <v>1345</v>
       </c>
       <c r="C3" s="2">
-        <v>461.5128173828125</v>
+        <v>467.06903076171875</v>
       </c>
       <c r="D3" s="2">
         <v>61</v>
       </c>
       <c r="E3" s="2">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -11223,10 +11322,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="2">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="C4" s="2">
-        <v>152.46456909179688</v>
+        <v>162.51716613769531</v>
       </c>
       <c r="D4" s="2">
         <v>5</v>
@@ -11240,16 +11339,16 @@
         <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>1542</v>
+        <v>1587</v>
       </c>
       <c r="C5" s="2">
-        <v>536.56805419921875</v>
+        <v>552.22662353515625</v>
       </c>
       <c r="D5" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E5" s="2">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -11257,16 +11356,16 @@
         <v>6</v>
       </c>
       <c r="B6" s="2">
-        <v>937</v>
+        <v>963</v>
       </c>
       <c r="C6" s="2">
-        <v>280.66665649414063</v>
+        <v>288.45462036132813</v>
       </c>
       <c r="D6" s="2">
         <v>33</v>
       </c>
       <c r="E6" s="2">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -11274,10 +11373,10 @@
         <v>28</v>
       </c>
       <c r="B7" s="2">
-        <v>817</v>
+        <v>839</v>
       </c>
       <c r="C7" s="2">
-        <v>624.57000732421875</v>
+        <v>641.38824462890625</v>
       </c>
       <c r="D7" s="2">
         <v>16</v>
@@ -11291,16 +11390,16 @@
         <v>8</v>
       </c>
       <c r="B8" s="2">
-        <v>1792</v>
+        <v>1857</v>
       </c>
       <c r="C8" s="2">
-        <v>492.85064697265625</v>
+        <v>510.72747802734375</v>
       </c>
       <c r="D8" s="2">
         <v>78</v>
       </c>
       <c r="E8" s="2">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -11308,10 +11407,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="2">
-        <v>421</v>
+        <v>440</v>
       </c>
       <c r="C9" s="2">
-        <v>171.52449035644531</v>
+        <v>179.2655029296875</v>
       </c>
       <c r="D9" s="2">
         <v>27</v>
@@ -11325,16 +11424,16 @@
         <v>10</v>
       </c>
       <c r="B10" s="2">
-        <v>935</v>
+        <v>950</v>
       </c>
       <c r="C10" s="2">
-        <v>464.09124755859375</v>
+        <v>471.53656005859375</v>
       </c>
       <c r="D10" s="2">
         <v>17</v>
       </c>
       <c r="E10" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -11342,16 +11441,16 @@
         <v>11</v>
       </c>
       <c r="B11" s="2">
-        <v>533</v>
+        <v>537</v>
       </c>
       <c r="C11" s="2">
-        <v>213.12071228027344</v>
+        <v>214.72012329101563</v>
       </c>
       <c r="D11" s="2">
         <v>40</v>
       </c>
       <c r="E11" s="2">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -11359,16 +11458,16 @@
         <v>12</v>
       </c>
       <c r="B12" s="2">
-        <v>2028</v>
+        <v>2088</v>
       </c>
       <c r="C12" s="2">
-        <v>147.18829345703125</v>
+        <v>151.54296875</v>
       </c>
       <c r="D12" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E12" s="2">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -11376,16 +11475,16 @@
         <v>13</v>
       </c>
       <c r="B13" s="2">
-        <v>14971</v>
+        <v>15173</v>
       </c>
       <c r="C13" s="2">
-        <v>629.8060302734375</v>
+        <v>638.30389404296875</v>
       </c>
       <c r="D13" s="2">
-        <v>828</v>
+        <v>835</v>
       </c>
       <c r="E13" s="2">
-        <v>2159</v>
+        <v>2178</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -11393,16 +11492,16 @@
         <v>14</v>
       </c>
       <c r="B14" s="2">
-        <v>1673</v>
+        <v>1675</v>
       </c>
       <c r="C14" s="2">
-        <v>562.27734375</v>
+        <v>562.94952392578125</v>
       </c>
       <c r="D14" s="2">
         <v>128</v>
       </c>
       <c r="E14" s="2">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -11410,16 +11509,16 @@
         <v>15</v>
       </c>
       <c r="B15" s="2">
-        <v>2262</v>
+        <v>2302</v>
       </c>
       <c r="C15" s="2">
-        <v>589.50311279296875</v>
+        <v>599.92755126953125</v>
       </c>
       <c r="D15" s="2">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="E15" s="2">
-        <v>185</v>
+        <v>191</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -11427,10 +11526,10 @@
         <v>16</v>
       </c>
       <c r="B16" s="2">
-        <v>662</v>
+        <v>678</v>
       </c>
       <c r="C16" s="2">
-        <v>234.40763854980469</v>
+        <v>240.07308959960938</v>
       </c>
       <c r="D16" s="2">
         <v>26</v>
@@ -11444,13 +11543,13 @@
         <v>17</v>
       </c>
       <c r="B17" s="2">
-        <v>539</v>
+        <v>548</v>
       </c>
       <c r="C17" s="2">
-        <v>198.35427856445313</v>
+        <v>201.66632080078125</v>
       </c>
       <c r="D17" s="2">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E17" s="2">
         <v>29</v>
@@ -11461,16 +11560,16 @@
         <v>18</v>
       </c>
       <c r="B18" s="2">
-        <v>905</v>
+        <v>929</v>
       </c>
       <c r="C18" s="2">
-        <v>368.86532592773438</v>
+        <v>378.64739990234375</v>
       </c>
       <c r="D18" s="2">
         <v>41</v>
       </c>
       <c r="E18" s="2">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -11478,10 +11577,10 @@
         <v>19</v>
       </c>
       <c r="B19" s="2">
-        <v>1527</v>
+        <v>1547</v>
       </c>
       <c r="C19" s="2">
-        <v>553.57177734375</v>
+        <v>560.82220458984375</v>
       </c>
       <c r="D19" s="2">
         <v>49</v>
@@ -11495,16 +11594,16 @@
         <v>29</v>
       </c>
       <c r="B20" s="2">
-        <v>8383</v>
+        <v>8608</v>
       </c>
       <c r="C20" s="2">
-        <v>485.72293090820313</v>
+        <v>498.759765625</v>
       </c>
       <c r="D20" s="2">
-        <v>360</v>
+        <v>367</v>
       </c>
       <c r="E20" s="2">
-        <v>604</v>
+        <v>631</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -11512,16 +11611,16 @@
         <v>21</v>
       </c>
       <c r="B21" s="2">
-        <v>1983</v>
+        <v>2016</v>
       </c>
       <c r="C21" s="2">
-        <v>650.57989501953125</v>
+        <v>661.406494140625</v>
       </c>
       <c r="D21" s="2">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E21" s="2">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -11529,17 +11628,23 @@
         <v>22</v>
       </c>
       <c r="B22" s="2">
-        <v>2287</v>
+        <v>2324</v>
       </c>
       <c r="C22" s="2">
-        <v>491.30496215820313</v>
+        <v>499.25347900390625</v>
       </c>
       <c r="D22" s="2">
         <v>102</v>
       </c>
       <c r="E22" s="2">
-        <v>198</v>
-      </c>
+        <v>201</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11548,15 +11653,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -11570,35 +11675,35 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>34</v>
       </c>
       <c r="B2" s="2">
-        <v>18352</v>
+        <v>18717</v>
       </c>
       <c r="C2" s="2">
-        <v>1627</v>
+        <v>1646</v>
       </c>
       <c r="D2" s="2">
-        <v>2588</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>2631</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>35</v>
       </c>
       <c r="B3" s="2">
-        <v>27571</v>
+        <v>28096</v>
       </c>
       <c r="C3" s="2">
-        <v>582</v>
+        <v>586</v>
       </c>
       <c r="D3" s="2">
-        <v>2129</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>2164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -11611,6 +11716,12 @@
       <c r="D4" s="2">
         <v>0</v>
       </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11623,10 +11734,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="13.08984375" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -11647,7 +11755,7 @@
         <v>38</v>
       </c>
       <c r="B2" s="2">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="C2" s="2">
         <v>5</v>
@@ -11661,7 +11769,7 @@
         <v>39</v>
       </c>
       <c r="B3" s="2">
-        <v>659</v>
+        <v>696</v>
       </c>
       <c r="C3" s="2">
         <v>9</v>
@@ -11675,7 +11783,7 @@
         <v>40</v>
       </c>
       <c r="B4" s="2">
-        <v>4631</v>
+        <v>4756</v>
       </c>
       <c r="C4" s="2">
         <v>81</v>
@@ -11689,10 +11797,10 @@
         <v>41</v>
       </c>
       <c r="B5" s="2">
-        <v>6165</v>
+        <v>6324</v>
       </c>
       <c r="C5" s="2">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D5" s="2">
         <v>12</v>
@@ -11703,10 +11811,10 @@
         <v>42</v>
       </c>
       <c r="B6" s="2">
-        <v>7236</v>
+        <v>7393</v>
       </c>
       <c r="C6" s="2">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="D6" s="2">
         <v>42</v>
@@ -11717,13 +11825,13 @@
         <v>43</v>
       </c>
       <c r="B7" s="2">
-        <v>8541</v>
+        <v>8706</v>
       </c>
       <c r="C7" s="2">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="D7" s="2">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -11731,13 +11839,13 @@
         <v>44</v>
       </c>
       <c r="B8" s="2">
-        <v>5425</v>
+        <v>5511</v>
       </c>
       <c r="C8" s="2">
-        <v>667</v>
+        <v>673</v>
       </c>
       <c r="D8" s="2">
-        <v>340</v>
+        <v>346</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -11745,13 +11853,13 @@
         <v>45</v>
       </c>
       <c r="B9" s="2">
-        <v>4508</v>
+        <v>4559</v>
       </c>
       <c r="C9" s="2">
-        <v>430</v>
+        <v>436</v>
       </c>
       <c r="D9" s="2">
-        <v>1031</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -11759,13 +11867,13 @@
         <v>46</v>
       </c>
       <c r="B10" s="2">
-        <v>5506</v>
+        <v>5575</v>
       </c>
       <c r="C10" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D10" s="2">
-        <v>1943</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -11773,13 +11881,13 @@
         <v>47</v>
       </c>
       <c r="B11" s="2">
-        <v>3017</v>
+        <v>3051</v>
       </c>
       <c r="C11" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11" s="2">
-        <v>1201</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -11805,9 +11913,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">

</xml_diff>